<commit_message>
Cargo distance edits from NEXT Group
</commit_message>
<xml_diff>
--- a/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
+++ b/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\trans\BCDTRtSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14573860-7D66-47A5-A492-02656B674ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{104BA830-36E9-4245-8929-7BFB63D69566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="791">
   <si>
     <t>Source:</t>
   </si>
@@ -2809,7 +2809,7 @@
     <numFmt numFmtId="169" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="170" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="68">
+  <fonts count="69">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3256,8 +3256,15 @@
       <name val="Inherit"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF444444"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3464,8 +3471,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="64">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -4264,6 +4277,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFB3B3B3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFB3B3B3"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFB3B3B3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF252525"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4525,7 +4553,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5012,6 +5040,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="68" fillId="40" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="40" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5039,14 +5079,17 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="33" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5054,15 +5097,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5920,7 +5954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6329,19 +6363,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="85" t="s">
@@ -6589,18 +6623,18 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="200" t="s">
+      <c r="A11" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="B11" s="199"/>
-      <c r="C11" s="199"/>
-      <c r="D11" s="199"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="199"/>
-      <c r="G11" s="199"/>
-      <c r="H11" s="199"/>
-      <c r="I11" s="199"/>
-      <c r="J11" s="199"/>
+      <c r="B11" s="201"/>
+      <c r="C11" s="201"/>
+      <c r="D11" s="201"/>
+      <c r="E11" s="201"/>
+      <c r="F11" s="201"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="201"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="201"/>
       <c r="K11" s="87">
         <v>44452.580524965277</v>
       </c>
@@ -6844,12 +6878,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="203" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="147"/>
@@ -7014,12 +7048,12 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="203" t="s">
         <v>420</v>
       </c>
-      <c r="B13" s="201"/>
-      <c r="C13" s="201"/>
-      <c r="D13" s="201"/>
+      <c r="B13" s="203"/>
+      <c r="C13" s="203"/>
+      <c r="D13" s="203"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="147"/>
@@ -7156,25 +7190,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6A2DD4-95F0-42B6-B835-D13B165F4574}">
   <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.42578125" style="6" customWidth="1"/>
-    <col min="2" max="5" width="28.42578125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="28.28515625" style="6" customWidth="1"/>
+    <col min="4" max="5" width="28.42578125" style="6" customWidth="1"/>
     <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="204" t="s">
         <v>493</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
     </row>
     <row r="2" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A2" s="92" t="s">
@@ -9151,18 +9186,19 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.42578125" style="6" customWidth="1"/>
-    <col min="2" max="5" width="28.42578125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="28.28515625" style="6" customWidth="1"/>
+    <col min="4" max="5" width="28.42578125" style="6" customWidth="1"/>
     <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="204" t="s">
         <v>650</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
     </row>
     <row r="2" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A2" s="92" t="s">
@@ -11496,18 +11532,19 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.42578125" style="6" customWidth="1"/>
-    <col min="2" max="5" width="28.42578125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="28.28515625" style="6" customWidth="1"/>
+    <col min="4" max="5" width="28.42578125" style="6" customWidth="1"/>
     <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="204" t="s">
         <v>611</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
     </row>
     <row r="2" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A2" s="92" t="s">
@@ -13613,7 +13650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564480E8-B5AD-440C-A1F7-B35A04FC90E9}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
@@ -14410,10 +14447,10 @@
       <c r="A37" s="48" t="s">
         <v>489</v>
       </c>
-      <c r="F37" s="197" t="s">
+      <c r="F37" s="199" t="s">
         <v>670</v>
       </c>
-      <c r="G37" s="197"/>
+      <c r="G37" s="199"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="84" t="s">
@@ -14736,10 +14773,10 @@
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="I53" s="197" t="s">
+      <c r="I53" s="199" t="s">
         <v>731</v>
       </c>
-      <c r="J53" s="197"/>
+      <c r="J53" s="199"/>
     </row>
     <row r="54" spans="1:10">
       <c r="I54" s="48" t="s">
@@ -14933,7 +14970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F81A32-6E09-4536-9605-3AE70AD9D670}">
   <dimension ref="A1:FA71"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
@@ -14947,9 +14984,9 @@
     <col min="6" max="6" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" style="6" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
@@ -19756,7 +19793,7 @@
       <c r="FA22" s="73"/>
     </row>
     <row r="23" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="205" t="s">
+      <c r="A23" s="207" t="s">
         <v>198</v>
       </c>
       <c r="B23" s="42" t="s">
@@ -19977,7 +20014,7 @@
       <c r="FA23" s="73"/>
     </row>
     <row r="24" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="206"/>
+      <c r="A24" s="208"/>
       <c r="B24" s="42" t="s">
         <v>197</v>
       </c>
@@ -20196,7 +20233,7 @@
       <c r="FA24" s="73"/>
     </row>
     <row r="25" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="206"/>
+      <c r="A25" s="208"/>
       <c r="B25" s="42" t="s">
         <v>390</v>
       </c>
@@ -20415,7 +20452,7 @@
       <c r="FA25" s="73"/>
     </row>
     <row r="26" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="206"/>
+      <c r="A26" s="208"/>
       <c r="B26" s="42" t="s">
         <v>196</v>
       </c>
@@ -20634,7 +20671,7 @@
       <c r="FA26" s="73"/>
     </row>
     <row r="27" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="207"/>
+      <c r="A27" s="209"/>
       <c r="B27" s="42" t="s">
         <v>195</v>
       </c>
@@ -20853,7 +20890,7 @@
       <c r="FA27" s="73"/>
     </row>
     <row r="28" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="205" t="s">
+      <c r="A28" s="207" t="s">
         <v>199</v>
       </c>
       <c r="B28" s="42" t="s">
@@ -21074,7 +21111,7 @@
       <c r="FA28" s="73"/>
     </row>
     <row r="29" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="206"/>
+      <c r="A29" s="208"/>
       <c r="B29" s="42" t="s">
         <v>196</v>
       </c>
@@ -21293,7 +21330,7 @@
       <c r="FA29" s="73"/>
     </row>
     <row r="30" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="207"/>
+      <c r="A30" s="209"/>
       <c r="B30" s="45" t="s">
         <v>195</v>
       </c>
@@ -21512,7 +21549,7 @@
       <c r="FA30" s="73"/>
     </row>
     <row r="31" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="204" t="s">
+      <c r="A31" s="206" t="s">
         <v>241</v>
       </c>
       <c r="B31" s="45" t="s">
@@ -21744,7 +21781,7 @@
       <c r="FA31" s="73"/>
     </row>
     <row r="32" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="204"/>
+      <c r="A32" s="206"/>
       <c r="B32" s="45" t="s">
         <v>391</v>
       </c>
@@ -21985,33 +22022,33 @@
       <c r="A34" s="67" t="s">
         <v>244</v>
       </c>
-      <c r="B34" s="209" t="s">
+      <c r="B34" s="211" t="s">
         <v>240</v>
       </c>
-      <c r="C34" s="209"/>
-      <c r="D34" s="209" t="s">
+      <c r="C34" s="211"/>
+      <c r="D34" s="211" t="s">
         <v>237</v>
       </c>
-      <c r="E34" s="209"/>
-      <c r="F34" s="209" t="s">
+      <c r="E34" s="211"/>
+      <c r="F34" s="211" t="s">
         <v>241</v>
       </c>
-      <c r="G34" s="209"/>
+      <c r="G34" s="211"/>
       <c r="I34" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="J34" s="210" t="s">
+      <c r="J34" s="212" t="s">
         <v>240</v>
       </c>
-      <c r="K34" s="210"/>
-      <c r="L34" s="208" t="s">
+      <c r="K34" s="212"/>
+      <c r="L34" s="210" t="s">
         <v>237</v>
       </c>
-      <c r="M34" s="208"/>
-      <c r="N34" s="208" t="s">
+      <c r="M34" s="210"/>
+      <c r="N34" s="210" t="s">
         <v>241</v>
       </c>
-      <c r="O34" s="208"/>
+      <c r="O34" s="210"/>
       <c r="P34" s="48"/>
       <c r="Q34" s="48"/>
       <c r="T34" s="48"/>
@@ -23725,20 +23762,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88A3E7C-5EE7-4C18-89A0-01D83214687A}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="99"/>
-    <col min="2" max="2" width="11.42578125" style="99" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="99" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.85546875" style="99" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11" style="99" bestFit="1" customWidth="1"/>
     <col min="8" max="13" width="11.85546875" style="99" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="10.42578125" style="99" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="10.28515625" style="99" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" style="99" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" style="99" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" style="99" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="11" style="99" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="9" style="99"/>
   </cols>
@@ -23749,72 +23786,72 @@
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="211"/>
-      <c r="C2" s="211" t="s">
+      <c r="B2" s="213"/>
+      <c r="C2" s="213" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
-      <c r="H2" s="211" t="s">
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+      <c r="H2" s="213" t="s">
         <v>671</v>
       </c>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
-      <c r="M2" s="211"/>
-      <c r="N2" s="211"/>
-      <c r="O2" s="211"/>
-      <c r="P2" s="211"/>
-      <c r="Q2" s="211" t="s">
+      <c r="I2" s="213"/>
+      <c r="J2" s="213"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="213"/>
+      <c r="M2" s="213"/>
+      <c r="N2" s="213"/>
+      <c r="O2" s="213"/>
+      <c r="P2" s="213"/>
+      <c r="Q2" s="213" t="s">
         <v>672</v>
       </c>
-      <c r="R2" s="211"/>
-      <c r="S2" s="211"/>
-      <c r="T2" s="211"/>
-      <c r="U2" s="211"/>
-      <c r="V2" s="211"/>
+      <c r="R2" s="213"/>
+      <c r="S2" s="213"/>
+      <c r="T2" s="213"/>
+      <c r="U2" s="213"/>
+      <c r="V2" s="213"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="211"/>
-      <c r="B3" s="211"/>
-      <c r="C3" s="211" t="s">
+      <c r="A3" s="213"/>
+      <c r="B3" s="213"/>
+      <c r="C3" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
-      <c r="H3" s="211" t="s">
+      <c r="D3" s="213"/>
+      <c r="E3" s="213"/>
+      <c r="F3" s="213"/>
+      <c r="G3" s="213"/>
+      <c r="H3" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="211"/>
-      <c r="J3" s="211"/>
-      <c r="K3" s="211" t="s">
+      <c r="I3" s="213"/>
+      <c r="J3" s="213"/>
+      <c r="K3" s="213" t="s">
         <v>673</v>
       </c>
-      <c r="L3" s="211"/>
-      <c r="M3" s="211"/>
-      <c r="N3" s="211" t="s">
+      <c r="L3" s="213"/>
+      <c r="M3" s="213"/>
+      <c r="N3" s="213" t="s">
         <v>674</v>
       </c>
-      <c r="O3" s="211"/>
-      <c r="P3" s="211"/>
-      <c r="Q3" s="211" t="s">
+      <c r="O3" s="213"/>
+      <c r="P3" s="213"/>
+      <c r="Q3" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="211"/>
-      <c r="S3" s="211"/>
-      <c r="T3" s="211" t="s">
+      <c r="R3" s="213"/>
+      <c r="S3" s="213"/>
+      <c r="T3" s="213" t="s">
         <v>675</v>
       </c>
-      <c r="U3" s="211"/>
-      <c r="V3" s="211"/>
+      <c r="U3" s="213"/>
+      <c r="V3" s="213"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="101" t="s">
@@ -23885,10 +23922,10 @@
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="211" t="s">
+      <c r="A5" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="211"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="102">
         <v>4080872227.8000002</v>
       </c>
@@ -23951,10 +23988,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A6" s="211" t="s">
+      <c r="A6" s="213" t="s">
         <v>682</v>
       </c>
-      <c r="B6" s="211"/>
+      <c r="B6" s="213"/>
       <c r="C6" s="106">
         <v>1655997518</v>
       </c>
@@ -24017,7 +24054,7 @@
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="211" t="s">
+      <c r="A7" s="213" t="s">
         <v>683</v>
       </c>
       <c r="B7" s="104" t="s">
@@ -24085,7 +24122,7 @@
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="211"/>
+      <c r="A8" s="213"/>
       <c r="B8" s="104" t="s">
         <v>685</v>
       </c>
@@ -24151,7 +24188,7 @@
       </c>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="211"/>
+      <c r="A9" s="213"/>
       <c r="B9" s="104" t="s">
         <v>686</v>
       </c>
@@ -24217,7 +24254,7 @@
       </c>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10" s="211"/>
+      <c r="A10" s="213"/>
       <c r="B10" s="104" t="s">
         <v>687</v>
       </c>
@@ -24283,7 +24320,7 @@
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="211"/>
+      <c r="A11" s="213"/>
       <c r="B11" s="104" t="s">
         <v>688</v>
       </c>
@@ -24349,7 +24386,7 @@
       </c>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="211"/>
+      <c r="A12" s="213"/>
       <c r="B12" s="104" t="s">
         <v>689</v>
       </c>
@@ -24415,7 +24452,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A13" s="211"/>
+      <c r="A13" s="213"/>
       <c r="B13" s="104" t="s">
         <v>690</v>
       </c>
@@ -24481,7 +24518,7 @@
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="211"/>
+      <c r="A14" s="213"/>
       <c r="B14" s="101" t="s">
         <v>691</v>
       </c>
@@ -24547,7 +24584,7 @@
       </c>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="211"/>
+      <c r="A15" s="213"/>
       <c r="B15" s="101" t="s">
         <v>692</v>
       </c>
@@ -24613,7 +24650,7 @@
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="211"/>
+      <c r="A16" s="213"/>
       <c r="B16" s="101" t="s">
         <v>693</v>
       </c>
@@ -24679,7 +24716,7 @@
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="211"/>
+      <c r="A17" s="213"/>
       <c r="B17" s="101" t="s">
         <v>694</v>
       </c>
@@ -24745,7 +24782,7 @@
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="211"/>
+      <c r="A18" s="213"/>
       <c r="B18" s="101" t="s">
         <v>695</v>
       </c>
@@ -24811,10 +24848,10 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A19" s="211" t="s">
+      <c r="A19" s="213" t="s">
         <v>696</v>
       </c>
-      <c r="B19" s="211"/>
+      <c r="B19" s="213"/>
       <c r="C19" s="106">
         <v>1510125438.8</v>
       </c>
@@ -24877,7 +24914,7 @@
       </c>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="211" t="s">
+      <c r="A20" s="213" t="s">
         <v>697</v>
       </c>
       <c r="B20" s="104" t="s">
@@ -24945,7 +24982,7 @@
       </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="211"/>
+      <c r="A21" s="213"/>
       <c r="B21" s="104" t="s">
         <v>685</v>
       </c>
@@ -25011,7 +25048,7 @@
       </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="211"/>
+      <c r="A22" s="213"/>
       <c r="B22" s="104" t="s">
         <v>686</v>
       </c>
@@ -25077,7 +25114,7 @@
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="211"/>
+      <c r="A23" s="213"/>
       <c r="B23" s="104" t="s">
         <v>687</v>
       </c>
@@ -25143,7 +25180,7 @@
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="211"/>
+      <c r="A24" s="213"/>
       <c r="B24" s="104" t="s">
         <v>688</v>
       </c>
@@ -25209,7 +25246,7 @@
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="211"/>
+      <c r="A25" s="213"/>
       <c r="B25" s="104" t="s">
         <v>689</v>
       </c>
@@ -25275,7 +25312,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A26" s="211"/>
+      <c r="A26" s="213"/>
       <c r="B26" s="104" t="s">
         <v>690</v>
       </c>
@@ -25341,7 +25378,7 @@
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="211"/>
+      <c r="A27" s="213"/>
       <c r="B27" s="101" t="s">
         <v>691</v>
       </c>
@@ -25407,7 +25444,7 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="211"/>
+      <c r="A28" s="213"/>
       <c r="B28" s="101" t="s">
         <v>692</v>
       </c>
@@ -25473,7 +25510,7 @@
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="211"/>
+      <c r="A29" s="213"/>
       <c r="B29" s="101" t="s">
         <v>693</v>
       </c>
@@ -25539,7 +25576,7 @@
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="211"/>
+      <c r="A30" s="213"/>
       <c r="B30" s="101" t="s">
         <v>694</v>
       </c>
@@ -25605,7 +25642,7 @@
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="211"/>
+      <c r="A31" s="213"/>
       <c r="B31" s="101" t="s">
         <v>695</v>
       </c>
@@ -25671,10 +25708,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A32" s="211" t="s">
+      <c r="A32" s="213" t="s">
         <v>698</v>
       </c>
-      <c r="B32" s="211"/>
+      <c r="B32" s="213"/>
       <c r="C32" s="106">
         <v>914749271</v>
       </c>
@@ -25737,7 +25774,7 @@
       </c>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="211" t="s">
+      <c r="A33" s="213" t="s">
         <v>699</v>
       </c>
       <c r="B33" s="104" t="s">
@@ -25805,7 +25842,7 @@
       </c>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="211"/>
+      <c r="A34" s="213"/>
       <c r="B34" s="104" t="s">
         <v>685</v>
       </c>
@@ -25871,7 +25908,7 @@
       </c>
     </row>
     <row r="35" spans="1:22">
-      <c r="A35" s="211"/>
+      <c r="A35" s="213"/>
       <c r="B35" s="104" t="s">
         <v>686</v>
       </c>
@@ -25937,7 +25974,7 @@
       </c>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="211"/>
+      <c r="A36" s="213"/>
       <c r="B36" s="104" t="s">
         <v>687</v>
       </c>
@@ -26003,7 +26040,7 @@
       </c>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="211"/>
+      <c r="A37" s="213"/>
       <c r="B37" s="104" t="s">
         <v>688</v>
       </c>
@@ -26069,7 +26106,7 @@
       </c>
     </row>
     <row r="38" spans="1:22">
-      <c r="A38" s="211"/>
+      <c r="A38" s="213"/>
       <c r="B38" s="104" t="s">
         <v>689</v>
       </c>
@@ -26135,7 +26172,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A39" s="211"/>
+      <c r="A39" s="213"/>
       <c r="B39" s="104" t="s">
         <v>690</v>
       </c>
@@ -26307,7 +26344,7 @@
   <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -28028,7 +28065,9 @@
   </sheetPr>
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -28146,128 +28185,128 @@
         <v>1</v>
       </c>
       <c r="C2" s="96">
-        <f>B2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.98688307386916851</v>
+        <f>B2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.0257544634651936</v>
       </c>
       <c r="D2" s="96">
-        <f>C2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.97393820148945875</v>
+        <f>C2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.0521722193187673</v>
       </c>
       <c r="E2" s="96">
-        <f>D2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.96116312604452669</v>
+        <f>D2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.079270350300304</v>
       </c>
       <c r="F2" s="96">
-        <f>E2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.94855562032052154</v>
+        <f>E2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.1070663791061799</v>
       </c>
       <c r="G2" s="96">
-        <f>F2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.93611348631779223</v>
+        <f>F2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.1355782797204141</v>
       </c>
       <c r="H2" s="96">
-        <f>G2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.92383455486768662</v>
+        <f>G2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.1648244890373409</v>
       </c>
       <c r="I2" s="96">
-        <f>H2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.91171668525437755</v>
+        <f>H2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.194823918783616</v>
       </c>
       <c r="J2" s="96">
-        <f>I2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.89975776484164938</v>
+        <f>I2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.2255959677472681</v>
       </c>
       <c r="K2" s="96">
-        <f>J2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.88795570870457941</v>
+        <f>J2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.2571605343217036</v>
       </c>
       <c r="L2" s="96">
-        <f>K2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.87630845926605128</v>
+        <f>K2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.2895380293727752</v>
       </c>
       <c r="M2" s="96">
-        <f>L2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.86481398593803571</v>
+        <f>L2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.322749389437234</v>
       </c>
       <c r="N2" s="96">
-        <f>M2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.85347028476757658</v>
+        <f>M2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.3568160902611024</v>
       </c>
       <c r="O2" s="96">
-        <f>N2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.84227537808742059</v>
+        <f>N2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.3917601606867187</v>
       </c>
       <c r="P2" s="96">
-        <f>O2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.83122731417122975</v>
+        <f>O2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.4276041968974369</v>
       </c>
       <c r="Q2" s="96">
-        <f>P2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.82032416689331622</v>
+        <f>P2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.4643713770291891</v>
       </c>
       <c r="R2" s="96">
-        <f>Q2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.80956403539284072</v>
+        <f>Q2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.5020854761583626</v>
       </c>
       <c r="S2" s="96">
-        <f>R2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.79894504374241493</v>
+        <f>R2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.5407708816756811</v>
       </c>
       <c r="T2" s="96">
-        <f>S2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.78846534062105178</v>
+        <f>S2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.5804526090560316</v>
       </c>
       <c r="U2" s="96">
-        <f>T2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.77812309899140453</v>
+        <f>T2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.6211563180344351</v>
       </c>
       <c r="V2" s="96">
-        <f>U2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.76791651578124065</v>
+        <f>U2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.6629083291986206</v>
       </c>
       <c r="W2" s="96">
-        <f>V2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.75784381156909264</v>
+        <f>V2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.7057356410089326</v>
       </c>
       <c r="X2" s="96">
-        <f>W2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.74790323027403305</v>
+        <f>W2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.7496659472565759</v>
       </c>
       <c r="Y2" s="96">
-        <f>X2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.73809303884951827</v>
+        <f>X2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.7947276549714888</v>
       </c>
       <c r="Z2" s="96">
-        <f>Y2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.72841152698124823</v>
+        <f>Y2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.8409499027914247</v>
       </c>
       <c r="AA2" s="96">
-        <f>Z2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.71885700678898901</v>
+        <f>Z2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.8883625798041181</v>
       </c>
       <c r="AB2" s="96">
-        <f>AA2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.70942781253230724</v>
+        <f>AA2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.9369963448747221</v>
       </c>
       <c r="AC2" s="96">
-        <f>AB2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.70012230032016365</v>
+        <f>AB2*(1+'DV-CAGR'!$N$82)</f>
+        <v>1.9868826464710116</v>
       </c>
       <c r="AD2" s="96">
-        <f>AC2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.69093884782431625</v>
+        <f>AC2*(1+'DV-CAGR'!$N$82)</f>
+        <v>2.0380537429991765</v>
       </c>
       <c r="AE2" s="96">
-        <f>AD2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.68187585399648287</v>
+        <f>AD2*(1+'DV-CAGR'!$N$82)</f>
+        <v>2.0905427236633498</v>
       </c>
       <c r="AF2" s="96">
-        <f>AE2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.67293173878921342</v>
+        <f>AE2*(1+'DV-CAGR'!$N$82)</f>
+        <v>2.1443835298623637</v>
       </c>
       <c r="AG2" s="96">
-        <f>AF2*(1+'DV-CAGR'!$N$72)</f>
-        <v>0.66410494288042332</v>
+        <f>AF2*(1+'DV-CAGR'!$N$82)</f>
+        <v>2.1996109771375667</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="95" customFormat="1">
@@ -28278,128 +28317,128 @@
         <v>1</v>
       </c>
       <c r="C3" s="96">
-        <f>B3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.98368801795707062</v>
+        <f>B3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.95480526999756732</v>
       </c>
       <c r="D3" s="96">
-        <f>C3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.96764211667231004</v>
+        <f>C3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.91165310361512741</v>
       </c>
       <c r="E3" s="96">
-        <f>D3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.95185795584116917</v>
+        <f>D3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.87045118774136199</v>
       </c>
       <c r="F3" s="96">
-        <f>E3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.93633126595806859</v>
+        <f>E3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.8311113813310943</v>
       </c>
       <c r="G3" s="96">
-        <f>F3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.92105784716152728</v>
+        <f>F3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.79354952684988667</v>
       </c>
       <c r="H3" s="96">
-        <f>G3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.90603356809812929</v>
+        <f>G3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.75768527024034782</v>
       </c>
       <c r="I3" s="96">
-        <f>H3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.8912543648050214</v>
+        <f>H3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.72344188902501505</v>
       </c>
       <c r="J3" s="96">
-        <f>I3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.87671623961063949</v>
+        <f>I3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.69074612817807968</v>
       </c>
       <c r="K3" s="96">
-        <f>J3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.86241526005336622</v>
+        <f>J3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.65952804341484561</v>
       </c>
       <c r="L3" s="96">
-        <f>K3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.84834755781782745</v>
+        <f>K3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.62972085156367896</v>
       </c>
       <c r="M3" s="96">
-        <f>L3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.83450932768854003</v>
+        <f>L3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.60126078770035651</v>
       </c>
       <c r="N3" s="96">
-        <f>M3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.82089682652062745</v>
+        <f>M3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.57408696873918885</v>
       </c>
       <c r="O3" s="96">
-        <f>N3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.80750637222732524</v>
+        <f>N3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.54814126318910616</v>
       </c>
       <c r="P3" s="96">
-        <f>O3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.79433434278400206</v>
+        <f>O3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.52336816679608211</v>
       </c>
       <c r="Q3" s="96">
-        <f>P3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.78137717524842731</v>
+        <f>P3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.49971468380586503</v>
       </c>
       <c r="R3" s="96">
-        <f>Q3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.7686313647970201</v>
+        <f>Q3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.47713021359300795</v>
       </c>
       <c r="S3" s="96">
-        <f>R3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.75609346377681885</v>
+        <f>R3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.45556644241366889</v>
       </c>
       <c r="T3" s="96">
-        <f>S3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.74376008077291511</v>
+        <f>S3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.43497724005061433</v>
       </c>
       <c r="U3" s="96">
-        <f>T3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.73162787969109966</v>
+        <f>T3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.41531856112932347</v>
       </c>
       <c r="V3" s="96">
-        <f>U3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.71969357885547192</v>
+        <f>U3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.39654835089408486</v>
       </c>
       <c r="W3" s="96">
-        <f>V3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.70795395012076989</v>
+        <f>V3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.37862645524251676</v>
       </c>
       <c r="X3" s="96">
-        <f>W3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.696405817999179</v>
+        <f>W3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.36151453482605306</v>
       </c>
       <c r="Y3" s="96">
-        <f>X3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.68504605880138481</v>
+        <f>X3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.34517598303263453</v>
       </c>
       <c r="Z3" s="96">
-        <f>Y3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.67387159979163702</v>
+        <f>Y3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.32957584767615034</v>
       </c>
       <c r="AA3" s="96">
-        <f>Z3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.6628794183565957</v>
+        <f>Z3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.31468075622510383</v>
       </c>
       <c r="AB3" s="96">
-        <f>AA3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.65206654118773544</v>
+        <f>AA3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.30045884441054893</v>
       </c>
       <c r="AC3" s="96">
-        <f>AB3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.64143004347708599</v>
+        <f>AB3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.28687968806057124</v>
       </c>
       <c r="AD3" s="96">
-        <f>AC3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.63096704812609239</v>
+        <f>AC3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.27391423801549158</v>
       </c>
       <c r="AE3" s="96">
-        <f>AD3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.62067472496737941</v>
+        <f>AD3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.26153475798455939</v>
       </c>
       <c r="AF3" s="96">
-        <f>AE3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.61055028999921135</v>
+        <f>AE3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.24971476521119565</v>
       </c>
       <c r="AG3" s="96">
-        <f>AF3*(1+'DV-CAGR'!$N$73)</f>
-        <v>0.60059100463243886</v>
+        <f>AF3*(1+'DV-CAGR'!$N$83)</f>
+        <v>0.23842897381985478</v>
       </c>
     </row>
     <row r="4" spans="1:33" s="95" customFormat="1">
@@ -28913,7 +28952,9 @@
   </sheetPr>
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -29032,128 +29073,128 @@
         <v>1</v>
       </c>
       <c r="C2" s="96">
-        <f>B2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.99043546689566553</v>
+        <f>B2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0042610726525127</v>
       </c>
       <c r="D2" s="96">
-        <f>C2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.98096241408483498</v>
+        <f>C2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0085403020451755</v>
       </c>
       <c r="E2" s="96">
-        <f>D2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.97157996660121271</v>
+        <f>D2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0128377655451772</v>
       </c>
       <c r="F2" s="96">
-        <f>E2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.96228725784714719</v>
+        <f>E2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0171535408493739</v>
       </c>
       <c r="G2" s="96">
-        <f>F2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.95308342951358893</v>
+        <f>F2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0214877059856937</v>
       </c>
       <c r="H2" s="96">
-        <f>G2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.94396763150081353</v>
+        <f>G2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0258403393145474</v>
       </c>
       <c r="I2" s="96">
-        <f>H2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.93493902183990385</v>
+        <f>H2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.030211519530245</v>
       </c>
       <c r="J2" s="96">
-        <f>I2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.92599676661498198</v>
+        <f>I2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0346013256624189</v>
       </c>
       <c r="K2" s="96">
-        <f>J2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.91714003988618631</v>
+        <f>J2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0390098370774525</v>
       </c>
       <c r="L2" s="96">
-        <f>K2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.9083680236133842</v>
+        <f>K2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0434371334799151</v>
       </c>
       <c r="M2" s="96">
-        <f>L2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.89967990758061511</v>
+        <f>L2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0478832949140027</v>
       </c>
       <c r="N2" s="96">
-        <f>M2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.89107488932125578</v>
+        <f>M2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0523484017649856</v>
       </c>
       <c r="O2" s="96">
-        <f>N2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.88255217404390141</v>
+        <f>N2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0568325347606617</v>
       </c>
       <c r="P2" s="96">
-        <f>O2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.87411097455895614</v>
+        <f>O2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0613357749728161</v>
       </c>
       <c r="Q2" s="96">
-        <f>P2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.86575051120592494</v>
+        <f>P2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0658582038186861</v>
       </c>
       <c r="R2" s="96">
-        <f>Q2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.85747001178140136</v>
+        <f>Q2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0703999030624343</v>
       </c>
       <c r="S2" s="96">
-        <f>R2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.84926871146774408</v>
+        <f>R2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0749609548166259</v>
       </c>
       <c r="T2" s="96">
-        <f>S2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.84114585276243536</v>
+        <f>S2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0795414415437141</v>
       </c>
       <c r="U2" s="96">
-        <f>T2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.83310068540811544</v>
+        <f>T2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0841414460575303</v>
       </c>
       <c r="V2" s="96">
-        <f>U2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.82513246632328574</v>
+        <f>U2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0887610515247816</v>
       </c>
       <c r="W2" s="96">
-        <f>V2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.81724045953367552</v>
+        <f>V2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.093400341466555</v>
       </c>
       <c r="X2" s="96">
-        <f>W2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.80942393610426422</v>
+        <f>W2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.0980593997598262</v>
       </c>
       <c r="Y2" s="96">
-        <f>X2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.8016821740719543</v>
+        <f>X2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1027383106389774</v>
       </c>
       <c r="Z2" s="96">
-        <f>Y2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.79401445837888829</v>
+        <f>Y2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1074371586973193</v>
       </c>
       <c r="AA2" s="96">
-        <f>Z2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.78642008080640324</v>
+        <f>Z2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1121560288886208</v>
       </c>
       <c r="AB2" s="96">
-        <f>AA2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.77889833990961699</v>
+        <f>AA2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1168950065286452</v>
       </c>
       <c r="AC2" s="96">
-        <f>AB2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.77144854095264026</v>
+        <f>AB2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1216541772966924</v>
       </c>
       <c r="AD2" s="96">
-        <f>AC2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.76406999584440816</v>
+        <f>AC2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.126433627237148</v>
       </c>
       <c r="AE2" s="96">
-        <f>AD2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.75676202307512563</v>
+        <f>AD2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1312334427610389</v>
       </c>
       <c r="AF2" s="96">
-        <f>AE2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.74952394765332042</v>
+        <f>AE2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1360537106475959</v>
       </c>
       <c r="AG2" s="96">
-        <f>AF2*(1+'DV-CAGR'!$N$74)</f>
-        <v>0.74235510104349878</v>
+        <f>AF2*(1+'DV-CAGR'!$N$84)</f>
+        <v>1.1408945180458219</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="95" customFormat="1">
@@ -29164,128 +29205,128 @@
         <v>1</v>
       </c>
       <c r="C3" s="96">
-        <f>B3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0097877219504034</v>
+        <f>B3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.0238834681230935</v>
       </c>
       <c r="D3" s="96">
-        <f>C3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0196712434017854</v>
+        <f>C3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.0483373562957738</v>
       </c>
       <c r="E3" s="96">
-        <f>D3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0296515020130241</v>
+        <f>D3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.0733752881271121</v>
       </c>
       <c r="F3" s="96">
-        <f>E3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.039729444620543</v>
+        <f>E3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.0990112126052123</v>
       </c>
       <c r="G3" s="96">
-        <f>F3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0499060273281362</v>
+        <f>F3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.1252594118683912</v>
       </c>
       <c r="H3" s="96">
-        <f>G3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0601822155976768</v>
+        <f>G3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.1521345091619608</v>
       </c>
       <c r="I3" s="96">
-        <f>H3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0705589843407095</v>
+        <f>H3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.1796514769850466</v>
       </c>
       <c r="J3" s="96">
-        <f>I3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0810373180109427</v>
+        <f>I3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.2078256454319791</v>
       </c>
       <c r="K3" s="96">
-        <f>J3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.0916182106976438</v>
+        <f>J3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.2366727107329085</v>
       </c>
       <c r="L3" s="96">
-        <f>K3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1023026662199493</v>
+        <f>K3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.2662087439983976</v>
       </c>
       <c r="M3" s="96">
-        <f>L3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1130916982220986</v>
+        <f>L3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.2964502001728655</v>
       </c>
       <c r="N3" s="96">
-        <f>M3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1239863302695989</v>
+        <f>M3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.3274139272018723</v>
       </c>
       <c r="O3" s="96">
-        <f>N3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.134987595946332</v>
+        <f>N3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.3591171754183486</v>
       </c>
       <c r="P3" s="96">
-        <f>O3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1460965389526117</v>
+        <f>O3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.3915776071530017</v>
       </c>
       <c r="Q3" s="96">
-        <f>P3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1573142132041996</v>
+        <f>P3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.4248133065742512</v>
       </c>
       <c r="R3" s="96">
-        <f>Q3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1686416829322923</v>
+        <f>Q3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.4588427897631768</v>
       </c>
       <c r="S3" s="96">
-        <f>R3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1800800227844852</v>
+        <f>R3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.4936850150290903</v>
       </c>
       <c r="T3" s="96">
-        <f>S3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.1916303179267256</v>
+        <f>S3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.52935939347148</v>
       </c>
       <c r="U3" s="96">
-        <f>T3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2032936641462633</v>
+        <f>T3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.5658857997942097</v>
       </c>
       <c r="V3" s="96">
-        <f>U3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.215071167955609</v>
+        <f>U3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.6032845833779994</v>
       </c>
       <c r="W3" s="96">
-        <f>V3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2269639466975104</v>
+        <f>V3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.6415765796173551</v>
       </c>
       <c r="X3" s="96">
-        <f>W3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2389731286509553</v>
+        <f>W3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.6807831215282631</v>
       </c>
       <c r="Y3" s="96">
-        <f>X3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2510998531382123</v>
+        <f>X3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.7209260516331171</v>
       </c>
       <c r="Z3" s="96">
-        <f>Y3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2633452706329196</v>
+        <f>Y3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.7620277341294979</v>
       </c>
       <c r="AA3" s="96">
-        <f>Z3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2757105428692317</v>
+        <f>Z3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.8041110673495864</v>
       </c>
       <c r="AB3" s="96">
-        <f>AA3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.2881968429520341</v>
+        <f>AA3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.8471994965171503</v>
       </c>
       <c r="AC3" s="96">
-        <f>AB3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.3008053554682362</v>
+        <f>AB3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.8913170268092121</v>
       </c>
       <c r="AD3" s="96">
-        <f>AC3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.3135372765991551</v>
+        <f>AC3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.9364882367296739</v>
       </c>
       <c r="AE3" s="96">
-        <f>AD3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.3263938142339977</v>
+        <f>AD3*(1+'DV-CAGR'!$N$85)</f>
+        <v>1.9827382918023526</v>
       </c>
       <c r="AF3" s="96">
-        <f>AE3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.3393761880844552</v>
+        <f>AE3*(1+'DV-CAGR'!$N$85)</f>
+        <v>2.0300929585910508</v>
       </c>
       <c r="AG3" s="96">
-        <f>AF3*(1+'DV-CAGR'!$N$75)</f>
-        <v>1.3524856298004171</v>
+        <f>AF3*(1+'DV-CAGR'!$N$85)</f>
+        <v>2.0785786190544768</v>
       </c>
     </row>
     <row r="4" spans="1:33" s="95" customFormat="1">
@@ -29840,40 +29881,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="186" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
     </row>
     <row r="2" spans="1:8" ht="25.5">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="187" t="s">
+      <c r="B2" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="187" t="s">
+      <c r="D2" s="180" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="F2" s="178" t="s">
+      <c r="F2" s="182" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="179"/>
+      <c r="G2" s="183"/>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A3" s="188"/>
-      <c r="B3" s="189"/>
-      <c r="C3" s="189"/>
-      <c r="D3" s="189"/>
+      <c r="A3" s="191"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
       <c r="E3" s="36" t="s">
         <v>11</v>
       </c>
@@ -29888,7 +29929,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" thickTop="1">
-      <c r="A4" s="183" t="s">
+      <c r="A4" s="187" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="35" t="s">
@@ -29907,10 +29948,10 @@
       <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="180" t="s">
+      <c r="B5" s="184" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="25" t="s">
@@ -29926,13 +29967,13 @@
       <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="184" t="s">
+      <c r="A6" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="185" t="s">
+      <c r="C6" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="25" t="s">
@@ -29945,13 +29986,13 @@
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="184" t="s">
+      <c r="A7" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="180" t="s">
+      <c r="B7" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="185" t="s">
+      <c r="C7" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="25" t="s">
@@ -29970,13 +30011,13 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="184" t="s">
+      <c r="A8" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="C8" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="25" t="s">
@@ -29992,13 +30033,13 @@
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="184" t="s">
+      <c r="A9" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="185" t="s">
+      <c r="C9" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -30014,13 +30055,13 @@
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="184" t="s">
+      <c r="A10" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="180" t="s">
+      <c r="B10" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="185" t="s">
+      <c r="C10" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="25" t="s">
@@ -30036,13 +30077,13 @@
       <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="184" t="s">
+      <c r="A11" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="180" t="s">
+      <c r="B11" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="185" t="s">
+      <c r="C11" s="189" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="25" t="s">
@@ -30055,13 +30096,13 @@
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="184" t="s">
+      <c r="A12" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="180" t="s">
+      <c r="B12" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="185" t="s">
+      <c r="C12" s="189" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="25" t="s">
@@ -30080,13 +30121,13 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="184" t="s">
+      <c r="A13" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="180" t="s">
+      <c r="B13" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="185" t="s">
+      <c r="C13" s="189" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="25" t="s">
@@ -30102,10 +30143,10 @@
       <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="184" t="s">
+      <c r="A14" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="180" t="s">
+      <c r="B14" s="184" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="25" t="s">
@@ -30127,10 +30168,10 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="184" t="s">
+      <c r="A15" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="180" t="s">
+      <c r="B15" s="184" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -30146,13 +30187,13 @@
       <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="184" t="s">
+      <c r="A16" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="185" t="s">
+      <c r="C16" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="25" t="s">
@@ -30165,13 +30206,13 @@
       <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="184" t="s">
+      <c r="A17" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="185" t="s">
+      <c r="C17" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="25" t="s">
@@ -30190,13 +30231,13 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="184" t="s">
+      <c r="A18" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="180" t="s">
+      <c r="B18" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="185" t="s">
+      <c r="C18" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="25" t="s">
@@ -30212,13 +30253,13 @@
       <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="184" t="s">
+      <c r="A19" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="180" t="s">
+      <c r="B19" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="185" t="s">
+      <c r="C19" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="25" t="s">
@@ -30234,10 +30275,10 @@
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A20" s="184" t="s">
+      <c r="A20" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="181" t="s">
+      <c r="B20" s="185" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="31" t="s">
@@ -30259,10 +30300,10 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="184" t="s">
+      <c r="A21" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="186" t="s">
+      <c r="B21" s="190" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="27" t="s">
@@ -30278,13 +30319,13 @@
       <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="184" t="s">
+      <c r="A22" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="180" t="s">
+      <c r="B22" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="185" t="s">
+      <c r="C22" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -30297,13 +30338,13 @@
       <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="184" t="s">
+      <c r="A23" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="180" t="s">
+      <c r="B23" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="185" t="s">
+      <c r="C23" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="25" t="s">
@@ -30322,13 +30363,13 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="184" t="s">
+      <c r="A24" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="180" t="s">
+      <c r="B24" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="185" t="s">
+      <c r="C24" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="25" t="s">
@@ -30344,13 +30385,13 @@
       <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="184" t="s">
+      <c r="A25" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="180" t="s">
+      <c r="B25" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="189" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="25" t="s">
@@ -30366,13 +30407,13 @@
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="184" t="s">
+      <c r="A26" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="180" t="s">
+      <c r="B26" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="185" t="s">
+      <c r="C26" s="189" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="25" t="s">
@@ -30385,13 +30426,13 @@
       <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="184" t="s">
+      <c r="A27" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="180" t="s">
+      <c r="B27" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="185" t="s">
+      <c r="C27" s="189" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="25" t="s">
@@ -30410,13 +30451,13 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="184" t="s">
+      <c r="A28" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="180" t="s">
+      <c r="B28" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="185" t="s">
+      <c r="C28" s="189" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="25" t="s">
@@ -30432,13 +30473,13 @@
       <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="184" t="s">
+      <c r="A29" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="180" t="s">
+      <c r="B29" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="185" t="s">
+      <c r="C29" s="189" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="25" t="s">
@@ -30454,13 +30495,13 @@
       <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="184" t="s">
+      <c r="A30" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="180" t="s">
+      <c r="B30" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="185" t="s">
+      <c r="C30" s="189" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="25" t="s">
@@ -30473,13 +30514,13 @@
       <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="184" t="s">
+      <c r="A31" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="180" t="s">
+      <c r="B31" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="185" t="s">
+      <c r="C31" s="189" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="25" t="s">
@@ -30501,13 +30542,13 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="184" t="s">
+      <c r="A32" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="180" t="s">
+      <c r="B32" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="185" t="s">
+      <c r="C32" s="189" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -30523,10 +30564,10 @@
       <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="184" t="s">
+      <c r="A33" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="180" t="s">
+      <c r="B33" s="184" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="25" t="s">
@@ -30548,10 +30589,10 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="184" t="s">
+      <c r="A34" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="180" t="s">
+      <c r="B34" s="184" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="25" t="s">
@@ -30567,10 +30608,10 @@
       <c r="G34" s="30"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="184" t="s">
+      <c r="A35" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="180" t="s">
+      <c r="B35" s="184" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="25" t="s">
@@ -30592,10 +30633,10 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="184" t="s">
+      <c r="A36" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="180" t="s">
+      <c r="B36" s="184" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="25" t="s">
@@ -30617,10 +30658,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A37" s="184" t="s">
+      <c r="A37" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="185" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="31" t="s">
@@ -30651,6 +30692,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B34:B37"/>
@@ -30666,8 +30709,6 @@
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30677,10 +30718,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8691AF6E-6FF3-4258-B536-2AC6D3469E02}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -30689,22 +30730,24 @@
     <col min="2" max="2" width="5.85546875" style="99" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="99" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" style="99" customWidth="1"/>
-    <col min="5" max="13" width="9" style="99" customWidth="1"/>
+    <col min="5" max="5" width="9" style="99" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="99" customWidth="1"/>
+    <col min="7" max="13" width="9" style="99" customWidth="1"/>
     <col min="14" max="15" width="9.85546875" style="99" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="99"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="195" t="s">
         <v>716</v>
       </c>
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="190" t="s">
+      <c r="C1" s="195" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="190" t="s">
+      <c r="D1" s="195" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="116" t="s">
@@ -30736,16 +30779,16 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="191" t="s">
+      <c r="A2" s="196" t="s">
         <v>716</v>
       </c>
-      <c r="B2" s="191" t="s">
+      <c r="B2" s="196" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="191" t="s">
+      <c r="C2" s="196" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="191" t="s">
+      <c r="D2" s="196" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="116" t="s">
@@ -30775,21 +30818,21 @@
       <c r="M2" s="171" t="s">
         <v>717</v>
       </c>
-      <c r="N2" s="192" t="s">
+      <c r="N2" s="197" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="196" t="s">
         <v>716</v>
       </c>
-      <c r="B3" s="191" t="s">
+      <c r="B3" s="196" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="191" t="s">
+      <c r="C3" s="196" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="191" t="s">
+      <c r="D3" s="196" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="116" t="s">
@@ -30819,7 +30862,7 @@
       <c r="M3" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="192"/>
+      <c r="N3" s="197"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="120" t="s">
@@ -32424,10 +32467,10 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="100" customFormat="1">
-      <c r="C40" s="197" t="s">
+      <c r="C40" s="199" t="s">
         <v>781</v>
       </c>
-      <c r="D40" s="197"/>
+      <c r="D40" s="199"/>
       <c r="E40" s="113">
         <f>E23</f>
         <v>43.7</v>
@@ -32470,8 +32513,8 @@
       </c>
     </row>
     <row r="41" spans="1:15" s="100" customFormat="1">
-      <c r="C41" s="197"/>
-      <c r="D41" s="197"/>
+      <c r="C41" s="199"/>
+      <c r="D41" s="199"/>
       <c r="E41" s="113">
         <f>E24</f>
         <v>53.3</v>
@@ -32514,8 +32557,8 @@
       </c>
     </row>
     <row r="42" spans="1:15" s="100" customFormat="1">
-      <c r="C42" s="197"/>
-      <c r="D42" s="197"/>
+      <c r="C42" s="199"/>
+      <c r="D42" s="199"/>
       <c r="E42" s="113">
         <f>E27</f>
         <v>19.899999999999999</v>
@@ -32558,8 +32601,8 @@
       </c>
     </row>
     <row r="43" spans="1:15" s="100" customFormat="1">
-      <c r="C43" s="197"/>
-      <c r="D43" s="197"/>
+      <c r="C43" s="199"/>
+      <c r="D43" s="199"/>
       <c r="E43" s="113">
         <f>E28</f>
         <v>20.399999999999999</v>
@@ -32602,8 +32645,8 @@
       </c>
     </row>
     <row r="44" spans="1:15" s="100" customFormat="1">
-      <c r="C44" s="197"/>
-      <c r="D44" s="197"/>
+      <c r="C44" s="199"/>
+      <c r="D44" s="199"/>
       <c r="E44" s="113">
         <f>E31</f>
         <v>39.299999999999997</v>
@@ -32646,8 +32689,8 @@
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="C45" s="197"/>
-      <c r="D45" s="197"/>
+      <c r="C45" s="199"/>
+      <c r="D45" s="199"/>
       <c r="E45" s="113">
         <f>E32</f>
         <v>41.1</v>
@@ -32690,8 +32733,8 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="C46" s="197"/>
-      <c r="D46" s="197"/>
+      <c r="C46" s="199"/>
+      <c r="D46" s="199"/>
       <c r="E46" s="113">
         <f>E36</f>
         <v>60</v>
@@ -32738,10 +32781,10 @@
       <c r="N47" s="40"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="C48" s="197" t="s">
+      <c r="C48" s="199" t="s">
         <v>782</v>
       </c>
-      <c r="D48" s="197"/>
+      <c r="D48" s="199"/>
       <c r="E48" s="113">
         <f t="shared" ref="E48:N48" si="14">E25</f>
         <v>130.9</v>
@@ -32784,8 +32827,8 @@
       </c>
     </row>
     <row r="49" spans="1:14" s="100" customFormat="1">
-      <c r="C49" s="197"/>
-      <c r="D49" s="197"/>
+      <c r="C49" s="199"/>
+      <c r="D49" s="199"/>
       <c r="E49" s="113">
         <f t="shared" ref="E49:N49" si="15">E29</f>
         <v>21.5</v>
@@ -32828,8 +32871,8 @@
       </c>
     </row>
     <row r="50" spans="1:14" s="100" customFormat="1">
-      <c r="C50" s="197"/>
-      <c r="D50" s="197"/>
+      <c r="C50" s="199"/>
+      <c r="D50" s="199"/>
       <c r="E50" s="113">
         <f t="shared" ref="E50:N50" si="16">E33</f>
         <v>56.7</v>
@@ -32872,8 +32915,8 @@
       </c>
     </row>
     <row r="51" spans="1:14" s="100" customFormat="1">
-      <c r="C51" s="197"/>
-      <c r="D51" s="197"/>
+      <c r="C51" s="199"/>
+      <c r="D51" s="199"/>
       <c r="E51" s="113">
         <f t="shared" ref="E51:N51" si="17">E35</f>
         <v>215.1</v>
@@ -32916,8 +32959,8 @@
       </c>
     </row>
     <row r="52" spans="1:14" s="100" customFormat="1">
-      <c r="C52" s="197"/>
-      <c r="D52" s="197"/>
+      <c r="C52" s="199"/>
+      <c r="D52" s="199"/>
       <c r="E52" s="113">
         <f t="shared" ref="E52:N52" si="18">E37</f>
         <v>28.7</v>
@@ -33006,7 +33049,7 @@
       </c>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="196" t="s">
+      <c r="A60" s="198" t="s">
         <v>783</v>
       </c>
       <c r="B60" s="132" t="s">
@@ -33058,7 +33101,7 @@
       </c>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="196"/>
+      <c r="A61" s="198"/>
       <c r="B61" s="135" t="s">
         <v>725</v>
       </c>
@@ -33108,7 +33151,7 @@
       </c>
     </row>
     <row r="62" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A62" s="196"/>
+      <c r="A62" s="198"/>
       <c r="B62" s="138" t="s">
         <v>726</v>
       </c>
@@ -33158,7 +33201,7 @@
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="196" t="s">
+      <c r="A63" s="198" t="s">
         <v>784</v>
       </c>
       <c r="B63" s="132" t="s">
@@ -33210,7 +33253,7 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="196"/>
+      <c r="A64" s="198"/>
       <c r="B64" s="135" t="s">
         <v>725</v>
       </c>
@@ -33259,8 +33302,8 @@
         <v>1426815</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
-      <c r="A65" s="196"/>
+    <row r="65" spans="1:15">
+      <c r="A65" s="198"/>
       <c r="B65" s="135" t="s">
         <v>725</v>
       </c>
@@ -33309,8 +33352,8 @@
         <v>1121099</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
-      <c r="A66" s="196"/>
+    <row r="66" spans="1:15">
+      <c r="A66" s="198"/>
       <c r="B66" s="135" t="s">
         <v>726</v>
       </c>
@@ -33359,8 +33402,8 @@
         <v>128549</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A67" s="196"/>
+    <row r="67" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A67" s="198"/>
       <c r="B67" s="138" t="s">
         <v>726</v>
       </c>
@@ -33409,9 +33452,9 @@
         <v>34815</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15.75" thickBot="1"/>
-    <row r="72" spans="1:14" ht="15.75" thickBot="1">
-      <c r="B72" s="193" t="s">
+    <row r="71" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="72" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B72" s="194" t="s">
         <v>778</v>
       </c>
       <c r="C72" s="133" t="s">
@@ -33459,8 +33502,8 @@
         <v>-1.3116926130831486E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" s="100" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B73" s="194"/>
+    <row r="73" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B73" s="193"/>
       <c r="C73" s="139" t="s">
         <v>729</v>
       </c>
@@ -33506,8 +33549,8 @@
         <v>-1.6311982042929385E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:14" s="100" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B74" s="195" t="s">
+    <row r="74" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B74" s="192" t="s">
         <v>779</v>
       </c>
       <c r="C74" s="70" t="s">
@@ -33555,8 +33598,8 @@
         <v>-9.5645331043344717E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="100" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B75" s="194"/>
+    <row r="75" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B75" s="193"/>
       <c r="C75" s="139" t="s">
         <v>729</v>
       </c>
@@ -33602,13 +33645,379 @@
         <v>9.7877219504034496E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:14" s="100" customFormat="1"/>
-    <row r="77" spans="1:14">
-      <c r="B77" s="48"/>
+    <row r="76" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1"/>
+    <row r="77" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B77" s="194" t="s">
+        <v>778</v>
+      </c>
+      <c r="C77" s="133" t="s">
+        <v>728</v>
+      </c>
+      <c r="D77" s="133"/>
+      <c r="E77" s="178">
+        <v>1458</v>
+      </c>
+      <c r="F77" s="178">
+        <v>1508</v>
+      </c>
+      <c r="G77" s="178">
+        <v>1575</v>
+      </c>
+      <c r="H77" s="178">
+        <v>1656</v>
+      </c>
+      <c r="I77" s="178">
+        <v>1734</v>
+      </c>
+      <c r="J77" s="178">
+        <v>1804</v>
+      </c>
+      <c r="K77" s="178">
+        <v>1868</v>
+      </c>
+      <c r="L77" s="178">
+        <v>1918</v>
+      </c>
+      <c r="M77" s="178">
+        <v>1986</v>
+      </c>
+      <c r="N77" s="175">
+        <f>(M77/E77)^(1/8)-1</f>
+        <v>3.938803960192172E-2</v>
+      </c>
+      <c r="O77" s="48"/>
+    </row>
+    <row r="78" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B78" s="193"/>
+      <c r="C78" s="139" t="s">
+        <v>729</v>
+      </c>
+      <c r="D78" s="133"/>
+      <c r="E78" s="179">
+        <v>99</v>
+      </c>
+      <c r="F78" s="179">
+        <v>97</v>
+      </c>
+      <c r="G78" s="179">
+        <v>95</v>
+      </c>
+      <c r="H78" s="179">
+        <v>92</v>
+      </c>
+      <c r="I78" s="179">
+        <v>89</v>
+      </c>
+      <c r="J78" s="179">
+        <v>87</v>
+      </c>
+      <c r="K78" s="179">
+        <v>84</v>
+      </c>
+      <c r="L78" s="179">
+        <v>81</v>
+      </c>
+      <c r="M78" s="179">
+        <v>78</v>
+      </c>
+      <c r="N78" s="175">
+        <f t="shared" ref="N78" si="39">(M78/E78)^(1/8)-1</f>
+        <v>-2.9361695407744359E-2</v>
+      </c>
+      <c r="O78" s="48"/>
+    </row>
+    <row r="79" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B79" s="192" t="s">
+        <v>779</v>
+      </c>
+      <c r="C79" s="70" t="s">
+        <v>728</v>
+      </c>
+      <c r="D79" s="133"/>
+      <c r="E79" s="179">
+        <v>324</v>
+      </c>
+      <c r="F79" s="179">
+        <v>329</v>
+      </c>
+      <c r="G79" s="179">
+        <v>335</v>
+      </c>
+      <c r="H79" s="179">
+        <v>343</v>
+      </c>
+      <c r="I79" s="179">
+        <v>349</v>
+      </c>
+      <c r="J79" s="179">
+        <v>354</v>
+      </c>
+      <c r="K79" s="179">
+        <v>359</v>
+      </c>
+      <c r="L79" s="179">
+        <v>359</v>
+      </c>
+      <c r="M79" s="179">
+        <v>362</v>
+      </c>
+      <c r="N79" s="175">
+        <f>(M79/E79)^(1/8)-1</f>
+        <v>1.3959118205026488E-2</v>
+      </c>
+      <c r="O79" s="48"/>
+    </row>
+    <row r="80" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B80" s="193"/>
+      <c r="C80" s="139" t="s">
+        <v>729</v>
+      </c>
+      <c r="D80" s="133"/>
+      <c r="E80" s="179">
+        <v>324</v>
+      </c>
+      <c r="F80" s="179">
+        <v>329</v>
+      </c>
+      <c r="G80" s="179">
+        <v>335</v>
+      </c>
+      <c r="H80" s="179">
+        <v>343</v>
+      </c>
+      <c r="I80" s="179">
+        <v>349</v>
+      </c>
+      <c r="J80" s="179">
+        <v>354</v>
+      </c>
+      <c r="K80" s="179">
+        <v>359</v>
+      </c>
+      <c r="L80" s="179">
+        <v>359</v>
+      </c>
+      <c r="M80" s="179">
+        <v>362</v>
+      </c>
+      <c r="N80" s="176">
+        <f t="shared" ref="N80" si="40">(M80/E80)^(1/8)-1</f>
+        <v>1.3959118205026488E-2</v>
+      </c>
+      <c r="O80" s="48"/>
+    </row>
+    <row r="81" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="48"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="48"/>
+      <c r="K81" s="48"/>
+      <c r="L81" s="48"/>
+      <c r="M81" s="48"/>
+      <c r="N81" s="48"/>
+      <c r="O81" s="48"/>
+    </row>
+    <row r="82" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B82" s="194" t="s">
+        <v>778</v>
+      </c>
+      <c r="C82" s="133" t="s">
+        <v>728</v>
+      </c>
+      <c r="D82" s="133"/>
+      <c r="E82" s="178">
+        <f>E72*E77</f>
+        <v>53286.743829686049</v>
+      </c>
+      <c r="F82" s="178">
+        <f t="shared" ref="F82:M82" si="41">F72*F77</f>
+        <v>52408.297290092356</v>
+      </c>
+      <c r="G82" s="178">
+        <f t="shared" si="41"/>
+        <v>55779.60766362938</v>
+      </c>
+      <c r="H82" s="178">
+        <f t="shared" si="41"/>
+        <v>57658.549995792979</v>
+      </c>
+      <c r="I82" s="178">
+        <f t="shared" si="41"/>
+        <v>60311.248652454895</v>
+      </c>
+      <c r="J82" s="178">
+        <f t="shared" si="41"/>
+        <v>61812.710884716653</v>
+      </c>
+      <c r="K82" s="178">
+        <f t="shared" si="41"/>
+        <v>63867.772731273457</v>
+      </c>
+      <c r="L82" s="178">
+        <f t="shared" si="41"/>
+        <v>64309.137872188789</v>
+      </c>
+      <c r="M82" s="178">
+        <f t="shared" si="41"/>
+        <v>65308.018372044789</v>
+      </c>
+      <c r="N82" s="175">
+        <f>(M82/E82)^(1/8)-1</f>
+        <v>2.5754463465193611E-2</v>
+      </c>
+      <c r="O82" s="48"/>
+    </row>
+    <row r="83" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B83" s="193"/>
+      <c r="C83" s="139" t="s">
+        <v>729</v>
+      </c>
+      <c r="D83" s="133"/>
+      <c r="E83" s="178">
+        <f t="shared" ref="E83:M83" si="42">E73*E78</f>
+        <v>4497.4396025194164</v>
+      </c>
+      <c r="F83" s="178">
+        <f t="shared" si="42"/>
+        <v>4208.3430257656883</v>
+      </c>
+      <c r="G83" s="178">
+        <f t="shared" si="42"/>
+        <v>4097.116103207748</v>
+      </c>
+      <c r="H83" s="178">
+        <f t="shared" si="42"/>
+        <v>3888.4070348595542</v>
+      </c>
+      <c r="I83" s="178">
+        <f t="shared" si="42"/>
+        <v>3769.7024799580599</v>
+      </c>
+      <c r="J83" s="178">
+        <f t="shared" si="42"/>
+        <v>3643.2113196980699</v>
+      </c>
+      <c r="K83" s="178">
+        <f t="shared" si="42"/>
+        <v>3497.9493076202889</v>
+      </c>
+      <c r="L83" s="178">
+        <f t="shared" si="42"/>
+        <v>3276.6076353792082</v>
+      </c>
+      <c r="M83" s="178">
+        <f t="shared" si="42"/>
+        <v>3106.588992155047</v>
+      </c>
+      <c r="N83" s="175">
+        <f t="shared" ref="N83" si="43">(M83/E83)^(1/8)-1</f>
+        <v>-4.5194730002432681E-2</v>
+      </c>
+      <c r="O83" s="48"/>
+    </row>
+    <row r="84" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B84" s="192" t="s">
+        <v>779</v>
+      </c>
+      <c r="C84" s="70" t="s">
+        <v>728</v>
+      </c>
+      <c r="D84" s="133"/>
+      <c r="E84" s="178">
+        <f t="shared" ref="E84:M84" si="44">E74*E79</f>
+        <v>14176.873480961749</v>
+      </c>
+      <c r="F84" s="178">
+        <f t="shared" si="44"/>
+        <v>14298.968917874234</v>
+      </c>
+      <c r="G84" s="178">
+        <f t="shared" si="44"/>
+        <v>14480.549757733557</v>
+      </c>
+      <c r="H84" s="178">
+        <f t="shared" si="44"/>
+        <v>15005.30291161387</v>
+      </c>
+      <c r="I84" s="178">
+        <f t="shared" si="44"/>
+        <v>15115.408033898173</v>
+      </c>
+      <c r="J84" s="178">
+        <f t="shared" si="44"/>
+        <v>15448.667900609029</v>
+      </c>
+      <c r="K84" s="178">
+        <f t="shared" si="44"/>
+        <v>15347.886968245761</v>
+      </c>
+      <c r="L84" s="178">
+        <f t="shared" si="44"/>
+        <v>14514.795849424441</v>
+      </c>
+      <c r="M84" s="178">
+        <f t="shared" si="44"/>
+        <v>14667.412097151402</v>
+      </c>
+      <c r="N84" s="175">
+        <f>(M84/E84)^(1/8)-1</f>
+        <v>4.2610726525127429E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B85" s="193"/>
+      <c r="C85" s="139" t="s">
+        <v>729</v>
+      </c>
+      <c r="D85" s="133"/>
+      <c r="E85" s="178">
+        <f t="shared" ref="E85:M85" si="45">E75*E80</f>
+        <v>24788.778793767851</v>
+      </c>
+      <c r="F85" s="178">
+        <f t="shared" si="45"/>
+        <v>25272.117646957464</v>
+      </c>
+      <c r="G85" s="178">
+        <f t="shared" si="45"/>
+        <v>25666.975432524672</v>
+      </c>
+      <c r="H85" s="178">
+        <f t="shared" si="45"/>
+        <v>26375.716124613384</v>
+      </c>
+      <c r="I85" s="178">
+        <f t="shared" si="45"/>
+        <v>27278.881969656504</v>
+      </c>
+      <c r="J85" s="178">
+        <f t="shared" si="45"/>
+        <v>28253.60517048063</v>
+      </c>
+      <c r="K85" s="178">
+        <f t="shared" si="45"/>
+        <v>27613.033618093359</v>
+      </c>
+      <c r="L85" s="178">
+        <f t="shared" si="45"/>
+        <v>30042.746371001984</v>
+      </c>
+      <c r="M85" s="178">
+        <f t="shared" si="45"/>
+        <v>29940.522746053222</v>
+      </c>
+      <c r="N85" s="176">
+        <f t="shared" ref="N85" si="46">(M85/E85)^(1/8)-1</f>
+        <v>2.3883468123093499E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="D1:D3"/>
+  <mergeCells count="15">
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="B74:B75"/>
@@ -33619,6 +34028,11 @@
     <mergeCell ref="A63:A67"/>
     <mergeCell ref="C40:D46"/>
     <mergeCell ref="C48:D52"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="D1:D3"/>
   </mergeCells>
   <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33639,29 +34053,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="199"/>
-      <c r="P1" s="199"/>
-      <c r="Q1" s="199"/>
-      <c r="R1" s="199"/>
-      <c r="S1" s="199"/>
-      <c r="T1" s="199"/>
-      <c r="U1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
+      <c r="R1" s="201"/>
+      <c r="S1" s="201"/>
+      <c r="T1" s="201"/>
+      <c r="U1" s="201"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="85" t="s">
@@ -34574,28 +34988,28 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="200" t="s">
+      <c r="A18" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="B18" s="199"/>
-      <c r="C18" s="199"/>
-      <c r="D18" s="199"/>
-      <c r="E18" s="199"/>
-      <c r="F18" s="199"/>
-      <c r="G18" s="199"/>
-      <c r="H18" s="199"/>
-      <c r="I18" s="199"/>
-      <c r="J18" s="199"/>
-      <c r="K18" s="199"/>
-      <c r="L18" s="199"/>
-      <c r="M18" s="199"/>
-      <c r="N18" s="199"/>
-      <c r="O18" s="199"/>
-      <c r="P18" s="199"/>
-      <c r="Q18" s="199"/>
-      <c r="R18" s="199"/>
-      <c r="S18" s="199"/>
-      <c r="T18" s="199"/>
+      <c r="B18" s="201"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="201"/>
+      <c r="E18" s="201"/>
+      <c r="F18" s="201"/>
+      <c r="G18" s="201"/>
+      <c r="H18" s="201"/>
+      <c r="I18" s="201"/>
+      <c r="J18" s="201"/>
+      <c r="K18" s="201"/>
+      <c r="L18" s="201"/>
+      <c r="M18" s="201"/>
+      <c r="N18" s="201"/>
+      <c r="O18" s="201"/>
+      <c r="P18" s="201"/>
+      <c r="Q18" s="201"/>
+      <c r="R18" s="201"/>
+      <c r="S18" s="201"/>
+      <c r="T18" s="201"/>
       <c r="U18" s="87">
         <v>44452.597080150474</v>
       </c>
@@ -34624,29 +35038,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="199"/>
-      <c r="P1" s="199"/>
-      <c r="Q1" s="199"/>
-      <c r="R1" s="199"/>
-      <c r="S1" s="199"/>
-      <c r="T1" s="199"/>
-      <c r="U1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
+      <c r="R1" s="201"/>
+      <c r="S1" s="201"/>
+      <c r="T1" s="201"/>
+      <c r="U1" s="201"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="85" t="s">
@@ -35559,28 +35973,28 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="200" t="s">
+      <c r="A18" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="B18" s="199"/>
-      <c r="C18" s="199"/>
-      <c r="D18" s="199"/>
-      <c r="E18" s="199"/>
-      <c r="F18" s="199"/>
-      <c r="G18" s="199"/>
-      <c r="H18" s="199"/>
-      <c r="I18" s="199"/>
-      <c r="J18" s="199"/>
-      <c r="K18" s="199"/>
-      <c r="L18" s="199"/>
-      <c r="M18" s="199"/>
-      <c r="N18" s="199"/>
-      <c r="O18" s="199"/>
-      <c r="P18" s="199"/>
-      <c r="Q18" s="199"/>
-      <c r="R18" s="199"/>
-      <c r="S18" s="199"/>
-      <c r="T18" s="199"/>
+      <c r="B18" s="201"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="201"/>
+      <c r="E18" s="201"/>
+      <c r="F18" s="201"/>
+      <c r="G18" s="201"/>
+      <c r="H18" s="201"/>
+      <c r="I18" s="201"/>
+      <c r="J18" s="201"/>
+      <c r="K18" s="201"/>
+      <c r="L18" s="201"/>
+      <c r="M18" s="201"/>
+      <c r="N18" s="201"/>
+      <c r="O18" s="201"/>
+      <c r="P18" s="201"/>
+      <c r="Q18" s="201"/>
+      <c r="R18" s="201"/>
+      <c r="S18" s="201"/>
+      <c r="T18" s="201"/>
       <c r="U18" s="87">
         <v>44452.596946840291</v>
       </c>
@@ -35609,29 +36023,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="199"/>
-      <c r="P1" s="199"/>
-      <c r="Q1" s="199"/>
-      <c r="R1" s="199"/>
-      <c r="S1" s="199"/>
-      <c r="T1" s="199"/>
-      <c r="U1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
+      <c r="R1" s="201"/>
+      <c r="S1" s="201"/>
+      <c r="T1" s="201"/>
+      <c r="U1" s="201"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="85" t="s">
@@ -36219,28 +36633,28 @@
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="200" t="s">
+      <c r="A13" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="B13" s="199"/>
-      <c r="C13" s="199"/>
-      <c r="D13" s="199"/>
-      <c r="E13" s="199"/>
-      <c r="F13" s="199"/>
-      <c r="G13" s="199"/>
-      <c r="H13" s="199"/>
-      <c r="I13" s="199"/>
-      <c r="J13" s="199"/>
-      <c r="K13" s="199"/>
-      <c r="L13" s="199"/>
-      <c r="M13" s="199"/>
-      <c r="N13" s="199"/>
-      <c r="O13" s="199"/>
-      <c r="P13" s="199"/>
-      <c r="Q13" s="199"/>
-      <c r="R13" s="199"/>
-      <c r="S13" s="199"/>
-      <c r="T13" s="199"/>
+      <c r="B13" s="201"/>
+      <c r="C13" s="201"/>
+      <c r="D13" s="201"/>
+      <c r="E13" s="201"/>
+      <c r="F13" s="201"/>
+      <c r="G13" s="201"/>
+      <c r="H13" s="201"/>
+      <c r="I13" s="201"/>
+      <c r="J13" s="201"/>
+      <c r="K13" s="201"/>
+      <c r="L13" s="201"/>
+      <c r="M13" s="201"/>
+      <c r="N13" s="201"/>
+      <c r="O13" s="201"/>
+      <c r="P13" s="201"/>
+      <c r="Q13" s="201"/>
+      <c r="R13" s="201"/>
+      <c r="S13" s="201"/>
+      <c r="T13" s="201"/>
       <c r="U13" s="87">
         <v>44452.596521967585</v>
       </c>
@@ -36269,19 +36683,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="85" t="s">
@@ -36809,18 +37223,18 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="B19" s="199"/>
-      <c r="C19" s="199"/>
-      <c r="D19" s="199"/>
-      <c r="E19" s="199"/>
-      <c r="F19" s="199"/>
-      <c r="G19" s="199"/>
-      <c r="H19" s="199"/>
-      <c r="I19" s="199"/>
-      <c r="J19" s="199"/>
+      <c r="B19" s="201"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="201"/>
+      <c r="E19" s="201"/>
+      <c r="F19" s="201"/>
+      <c r="G19" s="201"/>
+      <c r="H19" s="201"/>
+      <c r="I19" s="201"/>
+      <c r="J19" s="201"/>
       <c r="K19" s="87">
         <v>44452.580671828706</v>
       </c>
@@ -36854,19 +37268,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="85" t="s">
@@ -37394,18 +37808,18 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="B19" s="199"/>
-      <c r="C19" s="199"/>
-      <c r="D19" s="199"/>
-      <c r="E19" s="199"/>
-      <c r="F19" s="199"/>
-      <c r="G19" s="199"/>
-      <c r="H19" s="199"/>
-      <c r="I19" s="199"/>
-      <c r="J19" s="199"/>
+      <c r="B19" s="201"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="201"/>
+      <c r="E19" s="201"/>
+      <c r="F19" s="201"/>
+      <c r="G19" s="201"/>
+      <c r="H19" s="201"/>
+      <c r="I19" s="201"/>
+      <c r="J19" s="201"/>
       <c r="K19" s="87">
         <v>44452.580602870381</v>
       </c>

</xml_diff>

<commit_message>
Edit BCDTRtSY projections for onroad vehicles
</commit_message>
<xml_diff>
--- a/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
+++ b/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\trans\BCDTRtSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{104BA830-36E9-4245-8929-7BFB63D69566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB811A48-BEBB-4BF4-87BF-9DE5808B3A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="797">
   <si>
     <t>Source:</t>
   </si>
@@ -2792,6 +2792,24 @@
   <si>
     <t>증가율은 2020-&gt;2021 물량증가율인 약4.6%를 사용했으며, 2019년의 물량에 도달한 이후 기존 CAGR인 0.6%를 이용하여 2050년까지 데이터를 추정했다.</t>
     <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAGR</t>
+  </si>
+  <si>
+    <t>Average Annual Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on some basic curve fitting, we determined that extrapolating </t>
+  </si>
+  <si>
+    <t>passenger LDV, freight LDV, and freight HDV growth with a linear trend</t>
+  </si>
+  <si>
+    <t>was most fitting. However, for passenger HDVs we determined that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an exponential trend was most fitting. </t>
   </si>
 </sst>
 </file>
@@ -4553,7 +4571,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5046,6 +5064,9 @@
     <xf numFmtId="0" fontId="68" fillId="40" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="50" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5082,22 +5103,22 @@
     <xf numFmtId="0" fontId="50" fillId="33" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5143,6 +5164,9 @@
     </xf>
     <xf numFmtId="0" fontId="66" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="155">
@@ -5952,9 +5976,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O83"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6323,10 +6349,24 @@
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="161"/>
+      <c r="A82" s="161" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="161"/>
+      <c r="A83" s="161" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="151" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="151" t="s">
+        <v>796</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="42" type="noConversion"/>
@@ -6363,19 +6403,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="85" t="s">
@@ -6623,18 +6663,18 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="202" t="s">
+      <c r="A11" s="203" t="s">
         <v>419</v>
       </c>
-      <c r="B11" s="201"/>
-      <c r="C11" s="201"/>
-      <c r="D11" s="201"/>
-      <c r="E11" s="201"/>
-      <c r="F11" s="201"/>
-      <c r="G11" s="201"/>
-      <c r="H11" s="201"/>
-      <c r="I11" s="201"/>
-      <c r="J11" s="201"/>
+      <c r="B11" s="202"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="202"/>
+      <c r="E11" s="202"/>
+      <c r="F11" s="202"/>
+      <c r="G11" s="202"/>
+      <c r="H11" s="202"/>
+      <c r="I11" s="202"/>
+      <c r="J11" s="202"/>
       <c r="K11" s="87">
         <v>44452.580524965277</v>
       </c>
@@ -6878,12 +6918,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="204" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="147"/>
@@ -7048,12 +7088,12 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="203" t="s">
+      <c r="A13" s="204" t="s">
         <v>420</v>
       </c>
-      <c r="B13" s="203"/>
-      <c r="C13" s="203"/>
-      <c r="D13" s="203"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="147"/>
@@ -7203,13 +7243,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="205" t="s">
         <v>493</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
     </row>
     <row r="2" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A2" s="92" t="s">
@@ -9192,13 +9232,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="205" t="s">
         <v>650</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
     </row>
     <row r="2" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A2" s="92" t="s">
@@ -11538,13 +11578,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="205" t="s">
         <v>611</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
     </row>
     <row r="2" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A2" s="92" t="s">
@@ -14447,10 +14487,10 @@
       <c r="A37" s="48" t="s">
         <v>489</v>
       </c>
-      <c r="F37" s="199" t="s">
+      <c r="F37" s="200" t="s">
         <v>670</v>
       </c>
-      <c r="G37" s="199"/>
+      <c r="G37" s="200"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="84" t="s">
@@ -14773,10 +14813,10 @@
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="I53" s="199" t="s">
+      <c r="I53" s="200" t="s">
         <v>731</v>
       </c>
-      <c r="J53" s="199"/>
+      <c r="J53" s="200"/>
     </row>
     <row r="54" spans="1:10">
       <c r="I54" s="48" t="s">
@@ -19793,7 +19833,7 @@
       <c r="FA22" s="73"/>
     </row>
     <row r="23" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="207" t="s">
+      <c r="A23" s="208" t="s">
         <v>198</v>
       </c>
       <c r="B23" s="42" t="s">
@@ -20014,7 +20054,7 @@
       <c r="FA23" s="73"/>
     </row>
     <row r="24" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="208"/>
+      <c r="A24" s="209"/>
       <c r="B24" s="42" t="s">
         <v>197</v>
       </c>
@@ -20233,7 +20273,7 @@
       <c r="FA24" s="73"/>
     </row>
     <row r="25" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="208"/>
+      <c r="A25" s="209"/>
       <c r="B25" s="42" t="s">
         <v>390</v>
       </c>
@@ -20452,7 +20492,7 @@
       <c r="FA25" s="73"/>
     </row>
     <row r="26" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="208"/>
+      <c r="A26" s="209"/>
       <c r="B26" s="42" t="s">
         <v>196</v>
       </c>
@@ -20671,7 +20711,7 @@
       <c r="FA26" s="73"/>
     </row>
     <row r="27" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="209"/>
+      <c r="A27" s="210"/>
       <c r="B27" s="42" t="s">
         <v>195</v>
       </c>
@@ -20890,7 +20930,7 @@
       <c r="FA27" s="73"/>
     </row>
     <row r="28" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="207" t="s">
+      <c r="A28" s="208" t="s">
         <v>199</v>
       </c>
       <c r="B28" s="42" t="s">
@@ -21111,7 +21151,7 @@
       <c r="FA28" s="73"/>
     </row>
     <row r="29" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="208"/>
+      <c r="A29" s="209"/>
       <c r="B29" s="42" t="s">
         <v>196</v>
       </c>
@@ -21330,7 +21370,7 @@
       <c r="FA29" s="73"/>
     </row>
     <row r="30" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="209"/>
+      <c r="A30" s="210"/>
       <c r="B30" s="45" t="s">
         <v>195</v>
       </c>
@@ -21549,7 +21589,7 @@
       <c r="FA30" s="73"/>
     </row>
     <row r="31" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="206" t="s">
+      <c r="A31" s="207" t="s">
         <v>241</v>
       </c>
       <c r="B31" s="45" t="s">
@@ -21781,7 +21821,7 @@
       <c r="FA31" s="73"/>
     </row>
     <row r="32" spans="1:157" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="206"/>
+      <c r="A32" s="207"/>
       <c r="B32" s="45" t="s">
         <v>391</v>
       </c>
@@ -22022,33 +22062,33 @@
       <c r="A34" s="67" t="s">
         <v>244</v>
       </c>
-      <c r="B34" s="211" t="s">
+      <c r="B34" s="212" t="s">
         <v>240</v>
       </c>
-      <c r="C34" s="211"/>
-      <c r="D34" s="211" t="s">
+      <c r="C34" s="212"/>
+      <c r="D34" s="212" t="s">
         <v>237</v>
       </c>
-      <c r="E34" s="211"/>
-      <c r="F34" s="211" t="s">
+      <c r="E34" s="212"/>
+      <c r="F34" s="212" t="s">
         <v>241</v>
       </c>
-      <c r="G34" s="211"/>
+      <c r="G34" s="212"/>
       <c r="I34" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="J34" s="212" t="s">
+      <c r="J34" s="213" t="s">
         <v>240</v>
       </c>
-      <c r="K34" s="212"/>
-      <c r="L34" s="210" t="s">
+      <c r="K34" s="213"/>
+      <c r="L34" s="211" t="s">
         <v>237</v>
       </c>
-      <c r="M34" s="210"/>
-      <c r="N34" s="210" t="s">
+      <c r="M34" s="211"/>
+      <c r="N34" s="211" t="s">
         <v>241</v>
       </c>
-      <c r="O34" s="210"/>
+      <c r="O34" s="211"/>
       <c r="P34" s="48"/>
       <c r="Q34" s="48"/>
       <c r="T34" s="48"/>
@@ -23786,72 +23826,72 @@
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="214" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213" t="s">
+      <c r="B2" s="214"/>
+      <c r="C2" s="214" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
-      <c r="H2" s="213" t="s">
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214" t="s">
         <v>671</v>
       </c>
-      <c r="I2" s="213"/>
-      <c r="J2" s="213"/>
-      <c r="K2" s="213"/>
-      <c r="L2" s="213"/>
-      <c r="M2" s="213"/>
-      <c r="N2" s="213"/>
-      <c r="O2" s="213"/>
-      <c r="P2" s="213"/>
-      <c r="Q2" s="213" t="s">
+      <c r="I2" s="214"/>
+      <c r="J2" s="214"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="214"/>
+      <c r="M2" s="214"/>
+      <c r="N2" s="214"/>
+      <c r="O2" s="214"/>
+      <c r="P2" s="214"/>
+      <c r="Q2" s="214" t="s">
         <v>672</v>
       </c>
-      <c r="R2" s="213"/>
-      <c r="S2" s="213"/>
-      <c r="T2" s="213"/>
-      <c r="U2" s="213"/>
-      <c r="V2" s="213"/>
+      <c r="R2" s="214"/>
+      <c r="S2" s="214"/>
+      <c r="T2" s="214"/>
+      <c r="U2" s="214"/>
+      <c r="V2" s="214"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="213"/>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213" t="s">
+      <c r="A3" s="214"/>
+      <c r="B3" s="214"/>
+      <c r="C3" s="214" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="213"/>
-      <c r="E3" s="213"/>
-      <c r="F3" s="213"/>
-      <c r="G3" s="213"/>
-      <c r="H3" s="213" t="s">
+      <c r="D3" s="214"/>
+      <c r="E3" s="214"/>
+      <c r="F3" s="214"/>
+      <c r="G3" s="214"/>
+      <c r="H3" s="214" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="213"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="213" t="s">
+      <c r="I3" s="214"/>
+      <c r="J3" s="214"/>
+      <c r="K3" s="214" t="s">
         <v>673</v>
       </c>
-      <c r="L3" s="213"/>
-      <c r="M3" s="213"/>
-      <c r="N3" s="213" t="s">
+      <c r="L3" s="214"/>
+      <c r="M3" s="214"/>
+      <c r="N3" s="214" t="s">
         <v>674</v>
       </c>
-      <c r="O3" s="213"/>
-      <c r="P3" s="213"/>
-      <c r="Q3" s="213" t="s">
+      <c r="O3" s="214"/>
+      <c r="P3" s="214"/>
+      <c r="Q3" s="214" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="213"/>
-      <c r="S3" s="213"/>
-      <c r="T3" s="213" t="s">
+      <c r="R3" s="214"/>
+      <c r="S3" s="214"/>
+      <c r="T3" s="214" t="s">
         <v>675</v>
       </c>
-      <c r="U3" s="213"/>
-      <c r="V3" s="213"/>
+      <c r="U3" s="214"/>
+      <c r="V3" s="214"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="101" t="s">
@@ -23922,10 +23962,10 @@
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="213" t="s">
+      <c r="A5" s="214" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="213"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="102">
         <v>4080872227.8000002</v>
       </c>
@@ -23988,10 +24028,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A6" s="213" t="s">
+      <c r="A6" s="214" t="s">
         <v>682</v>
       </c>
-      <c r="B6" s="213"/>
+      <c r="B6" s="214"/>
       <c r="C6" s="106">
         <v>1655997518</v>
       </c>
@@ -24054,7 +24094,7 @@
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="213" t="s">
+      <c r="A7" s="214" t="s">
         <v>683</v>
       </c>
       <c r="B7" s="104" t="s">
@@ -24122,7 +24162,7 @@
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="213"/>
+      <c r="A8" s="214"/>
       <c r="B8" s="104" t="s">
         <v>685</v>
       </c>
@@ -24188,7 +24228,7 @@
       </c>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="213"/>
+      <c r="A9" s="214"/>
       <c r="B9" s="104" t="s">
         <v>686</v>
       </c>
@@ -24254,7 +24294,7 @@
       </c>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10" s="213"/>
+      <c r="A10" s="214"/>
       <c r="B10" s="104" t="s">
         <v>687</v>
       </c>
@@ -24320,7 +24360,7 @@
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="213"/>
+      <c r="A11" s="214"/>
       <c r="B11" s="104" t="s">
         <v>688</v>
       </c>
@@ -24386,7 +24426,7 @@
       </c>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="213"/>
+      <c r="A12" s="214"/>
       <c r="B12" s="104" t="s">
         <v>689</v>
       </c>
@@ -24452,7 +24492,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A13" s="213"/>
+      <c r="A13" s="214"/>
       <c r="B13" s="104" t="s">
         <v>690</v>
       </c>
@@ -24518,7 +24558,7 @@
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="213"/>
+      <c r="A14" s="214"/>
       <c r="B14" s="101" t="s">
         <v>691</v>
       </c>
@@ -24584,7 +24624,7 @@
       </c>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="213"/>
+      <c r="A15" s="214"/>
       <c r="B15" s="101" t="s">
         <v>692</v>
       </c>
@@ -24650,7 +24690,7 @@
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="213"/>
+      <c r="A16" s="214"/>
       <c r="B16" s="101" t="s">
         <v>693</v>
       </c>
@@ -24716,7 +24756,7 @@
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="213"/>
+      <c r="A17" s="214"/>
       <c r="B17" s="101" t="s">
         <v>694</v>
       </c>
@@ -24782,7 +24822,7 @@
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="213"/>
+      <c r="A18" s="214"/>
       <c r="B18" s="101" t="s">
         <v>695</v>
       </c>
@@ -24848,10 +24888,10 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="214" t="s">
         <v>696</v>
       </c>
-      <c r="B19" s="213"/>
+      <c r="B19" s="214"/>
       <c r="C19" s="106">
         <v>1510125438.8</v>
       </c>
@@ -24914,7 +24954,7 @@
       </c>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="213" t="s">
+      <c r="A20" s="214" t="s">
         <v>697</v>
       </c>
       <c r="B20" s="104" t="s">
@@ -24982,7 +25022,7 @@
       </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="213"/>
+      <c r="A21" s="214"/>
       <c r="B21" s="104" t="s">
         <v>685</v>
       </c>
@@ -25048,7 +25088,7 @@
       </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="213"/>
+      <c r="A22" s="214"/>
       <c r="B22" s="104" t="s">
         <v>686</v>
       </c>
@@ -25114,7 +25154,7 @@
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="213"/>
+      <c r="A23" s="214"/>
       <c r="B23" s="104" t="s">
         <v>687</v>
       </c>
@@ -25180,7 +25220,7 @@
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="213"/>
+      <c r="A24" s="214"/>
       <c r="B24" s="104" t="s">
         <v>688</v>
       </c>
@@ -25246,7 +25286,7 @@
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="213"/>
+      <c r="A25" s="214"/>
       <c r="B25" s="104" t="s">
         <v>689</v>
       </c>
@@ -25312,7 +25352,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A26" s="213"/>
+      <c r="A26" s="214"/>
       <c r="B26" s="104" t="s">
         <v>690</v>
       </c>
@@ -25378,7 +25418,7 @@
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="213"/>
+      <c r="A27" s="214"/>
       <c r="B27" s="101" t="s">
         <v>691</v>
       </c>
@@ -25444,7 +25484,7 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="213"/>
+      <c r="A28" s="214"/>
       <c r="B28" s="101" t="s">
         <v>692</v>
       </c>
@@ -25510,7 +25550,7 @@
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="213"/>
+      <c r="A29" s="214"/>
       <c r="B29" s="101" t="s">
         <v>693</v>
       </c>
@@ -25576,7 +25616,7 @@
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="213"/>
+      <c r="A30" s="214"/>
       <c r="B30" s="101" t="s">
         <v>694</v>
       </c>
@@ -25642,7 +25682,7 @@
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="213"/>
+      <c r="A31" s="214"/>
       <c r="B31" s="101" t="s">
         <v>695</v>
       </c>
@@ -25708,10 +25748,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A32" s="213" t="s">
+      <c r="A32" s="214" t="s">
         <v>698</v>
       </c>
-      <c r="B32" s="213"/>
+      <c r="B32" s="214"/>
       <c r="C32" s="106">
         <v>914749271</v>
       </c>
@@ -25774,7 +25814,7 @@
       </c>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="213" t="s">
+      <c r="A33" s="214" t="s">
         <v>699</v>
       </c>
       <c r="B33" s="104" t="s">
@@ -25842,7 +25882,7 @@
       </c>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="213"/>
+      <c r="A34" s="214"/>
       <c r="B34" s="104" t="s">
         <v>685</v>
       </c>
@@ -25908,7 +25948,7 @@
       </c>
     </row>
     <row r="35" spans="1:22">
-      <c r="A35" s="213"/>
+      <c r="A35" s="214"/>
       <c r="B35" s="104" t="s">
         <v>686</v>
       </c>
@@ -25974,7 +26014,7 @@
       </c>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="213"/>
+      <c r="A36" s="214"/>
       <c r="B36" s="104" t="s">
         <v>687</v>
       </c>
@@ -26040,7 +26080,7 @@
       </c>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="213"/>
+      <c r="A37" s="214"/>
       <c r="B37" s="104" t="s">
         <v>688</v>
       </c>
@@ -26106,7 +26146,7 @@
       </c>
     </row>
     <row r="38" spans="1:22">
-      <c r="A38" s="213"/>
+      <c r="A38" s="214"/>
       <c r="B38" s="104" t="s">
         <v>689</v>
       </c>
@@ -26172,7 +26212,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A39" s="213"/>
+      <c r="A39" s="214"/>
       <c r="B39" s="104" t="s">
         <v>690</v>
       </c>
@@ -26312,13 +26352,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:A31"/>
-    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:P2"/>
@@ -26329,6 +26362,13 @@
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="T3:V3"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:A18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:A31"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28066,7 +28106,7 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -28185,128 +28225,128 @@
         <v>1</v>
       </c>
       <c r="C2" s="96">
-        <f>B2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.0257544634651936</v>
+        <f>$B$2*'DV-CAGR'!F89/'DV-CAGR'!$E$89</f>
+        <v>1.0233661866340256</v>
       </c>
       <c r="D2" s="96">
-        <f>C2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.0521722193187673</v>
+        <f>$B$2*'DV-CAGR'!G89/'DV-CAGR'!$E$89</f>
+        <v>1.0467323732680509</v>
       </c>
       <c r="E2" s="96">
-        <f>D2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.079270350300304</v>
+        <f>$B$2*'DV-CAGR'!H89/'DV-CAGR'!$E$89</f>
+        <v>1.0700985599020765</v>
       </c>
       <c r="F2" s="96">
-        <f>E2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.1070663791061799</v>
+        <f>$B$2*'DV-CAGR'!I89/'DV-CAGR'!$E$89</f>
+        <v>1.0934647465361018</v>
       </c>
       <c r="G2" s="96">
-        <f>F2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.1355782797204141</v>
+        <f>$B$2*'DV-CAGR'!J89/'DV-CAGR'!$E$89</f>
+        <v>1.1168309331701274</v>
       </c>
       <c r="H2" s="96">
-        <f>G2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.1648244890373409</v>
+        <f>$B$2*'DV-CAGR'!K89/'DV-CAGR'!$E$89</f>
+        <v>1.1401971198041527</v>
       </c>
       <c r="I2" s="96">
-        <f>H2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.194823918783616</v>
+        <f>$B$2*'DV-CAGR'!L89/'DV-CAGR'!$E$89</f>
+        <v>1.1635633064381783</v>
       </c>
       <c r="J2" s="96">
-        <f>I2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.2255959677472681</v>
+        <f>$B$2*'DV-CAGR'!M89/'DV-CAGR'!$E$89</f>
+        <v>1.1869294930722036</v>
       </c>
       <c r="K2" s="96">
-        <f>J2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.2571605343217036</v>
+        <f>$B$2*'DV-CAGR'!N89/'DV-CAGR'!$E$89</f>
+        <v>1.2102956797062292</v>
       </c>
       <c r="L2" s="96">
-        <f>K2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.2895380293727752</v>
+        <f>$B$2*'DV-CAGR'!O89/'DV-CAGR'!$E$89</f>
+        <v>1.2336618663402545</v>
       </c>
       <c r="M2" s="96">
-        <f>L2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.322749389437234</v>
+        <f>$B$2*'DV-CAGR'!P89/'DV-CAGR'!$E$89</f>
+        <v>1.2570280529742801</v>
       </c>
       <c r="N2" s="96">
-        <f>M2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.3568160902611024</v>
+        <f>$B$2*'DV-CAGR'!Q89/'DV-CAGR'!$E$89</f>
+        <v>1.2803942396083055</v>
       </c>
       <c r="O2" s="96">
-        <f>N2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.3917601606867187</v>
+        <f>$B$2*'DV-CAGR'!R89/'DV-CAGR'!$E$89</f>
+        <v>1.303760426242331</v>
       </c>
       <c r="P2" s="96">
-        <f>O2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.4276041968974369</v>
+        <f>$B$2*'DV-CAGR'!S89/'DV-CAGR'!$E$89</f>
+        <v>1.3271266128763564</v>
       </c>
       <c r="Q2" s="96">
-        <f>P2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.4643713770291891</v>
+        <f>$B$2*'DV-CAGR'!T89/'DV-CAGR'!$E$89</f>
+        <v>1.3504927995103819</v>
       </c>
       <c r="R2" s="96">
-        <f>Q2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.5020854761583626</v>
+        <f>$B$2*'DV-CAGR'!U89/'DV-CAGR'!$E$89</f>
+        <v>1.3738589861444073</v>
       </c>
       <c r="S2" s="96">
-        <f>R2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.5407708816756811</v>
+        <f>$B$2*'DV-CAGR'!V89/'DV-CAGR'!$E$89</f>
+        <v>1.3972251727784328</v>
       </c>
       <c r="T2" s="96">
-        <f>S2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.5804526090560316</v>
+        <f>$B$2*'DV-CAGR'!W89/'DV-CAGR'!$E$89</f>
+        <v>1.4205913594124582</v>
       </c>
       <c r="U2" s="96">
-        <f>T2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.6211563180344351</v>
+        <f>$B$2*'DV-CAGR'!X89/'DV-CAGR'!$E$89</f>
+        <v>1.4439575460464837</v>
       </c>
       <c r="V2" s="96">
-        <f>U2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.6629083291986206</v>
+        <f>$B$2*'DV-CAGR'!Y89/'DV-CAGR'!$E$89</f>
+        <v>1.4673237326805091</v>
       </c>
       <c r="W2" s="96">
-        <f>V2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.7057356410089326</v>
+        <f>$B$2*'DV-CAGR'!Z89/'DV-CAGR'!$E$89</f>
+        <v>1.4906899193145347</v>
       </c>
       <c r="X2" s="96">
-        <f>W2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.7496659472565759</v>
+        <f>$B$2*'DV-CAGR'!AA89/'DV-CAGR'!$E$89</f>
+        <v>1.51405610594856</v>
       </c>
       <c r="Y2" s="96">
-        <f>X2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.7947276549714888</v>
+        <f>$B$2*'DV-CAGR'!AB89/'DV-CAGR'!$E$89</f>
+        <v>1.5374222925825856</v>
       </c>
       <c r="Z2" s="96">
-        <f>Y2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.8409499027914247</v>
+        <f>$B$2*'DV-CAGR'!AC89/'DV-CAGR'!$E$89</f>
+        <v>1.5607884792166109</v>
       </c>
       <c r="AA2" s="96">
-        <f>Z2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.8883625798041181</v>
+        <f>$B$2*'DV-CAGR'!AD89/'DV-CAGR'!$E$89</f>
+        <v>1.5841546658506365</v>
       </c>
       <c r="AB2" s="96">
-        <f>AA2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.9369963448747221</v>
+        <f>$B$2*'DV-CAGR'!AE89/'DV-CAGR'!$E$89</f>
+        <v>1.6075208524846618</v>
       </c>
       <c r="AC2" s="96">
-        <f>AB2*(1+'DV-CAGR'!$N$82)</f>
-        <v>1.9868826464710116</v>
+        <f>$B$2*'DV-CAGR'!AF89/'DV-CAGR'!$E$89</f>
+        <v>1.6308870391186874</v>
       </c>
       <c r="AD2" s="96">
-        <f>AC2*(1+'DV-CAGR'!$N$82)</f>
-        <v>2.0380537429991765</v>
+        <f>$B$2*'DV-CAGR'!AG89/'DV-CAGR'!$E$89</f>
+        <v>1.6542532257527127</v>
       </c>
       <c r="AE2" s="96">
-        <f>AD2*(1+'DV-CAGR'!$N$82)</f>
-        <v>2.0905427236633498</v>
+        <f>$B$2*'DV-CAGR'!AH89/'DV-CAGR'!$E$89</f>
+        <v>1.6776194123867383</v>
       </c>
       <c r="AF2" s="96">
-        <f>AE2*(1+'DV-CAGR'!$N$82)</f>
-        <v>2.1443835298623637</v>
+        <f>$B$2*'DV-CAGR'!AI89/'DV-CAGR'!$E$89</f>
+        <v>1.7009855990207636</v>
       </c>
       <c r="AG2" s="96">
-        <f>AF2*(1+'DV-CAGR'!$N$82)</f>
-        <v>2.1996109771375667</v>
+        <f>$B$2*'DV-CAGR'!AJ89/'DV-CAGR'!$E$89</f>
+        <v>1.7243517856547892</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="95" customFormat="1">
@@ -28953,7 +28993,7 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C3" sqref="C3:AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -29073,128 +29113,128 @@
         <v>1</v>
       </c>
       <c r="C2" s="96">
-        <f>B2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0042610726525127</v>
+        <f>$B$2*'DV-CAGR'!F91/'DV-CAGR'!$E$91</f>
+        <v>1.0042244705099408</v>
       </c>
       <c r="D2" s="96">
-        <f>C2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0085403020451755</v>
+        <f>$B$2*'DV-CAGR'!G91/'DV-CAGR'!$E$91</f>
+        <v>1.0084489410198818</v>
       </c>
       <c r="E2" s="96">
-        <f>D2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0128377655451772</v>
+        <f>$B$2*'DV-CAGR'!H91/'DV-CAGR'!$E$91</f>
+        <v>1.0126734115298226</v>
       </c>
       <c r="F2" s="96">
-        <f>E2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0171535408493739</v>
+        <f>$B$2*'DV-CAGR'!I91/'DV-CAGR'!$E$91</f>
+        <v>1.0168978820397634</v>
       </c>
       <c r="G2" s="96">
-        <f>F2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0214877059856937</v>
+        <f>$B$2*'DV-CAGR'!J91/'DV-CAGR'!$E$91</f>
+        <v>1.0211223525497044</v>
       </c>
       <c r="H2" s="96">
-        <f>G2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0258403393145474</v>
+        <f>$B$2*'DV-CAGR'!K91/'DV-CAGR'!$E$91</f>
+        <v>1.0253468230596452</v>
       </c>
       <c r="I2" s="96">
-        <f>H2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.030211519530245</v>
+        <f>$B$2*'DV-CAGR'!L91/'DV-CAGR'!$E$91</f>
+        <v>1.0295712935695862</v>
       </c>
       <c r="J2" s="96">
-        <f>I2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0346013256624189</v>
+        <f>$B$2*'DV-CAGR'!M91/'DV-CAGR'!$E$91</f>
+        <v>1.033795764079527</v>
       </c>
       <c r="K2" s="96">
-        <f>J2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0390098370774525</v>
+        <f>$B$2*'DV-CAGR'!N91/'DV-CAGR'!$E$91</f>
+        <v>1.0380202345894678</v>
       </c>
       <c r="L2" s="96">
-        <f>K2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0434371334799151</v>
+        <f>$B$2*'DV-CAGR'!O91/'DV-CAGR'!$E$91</f>
+        <v>1.0422447050994088</v>
       </c>
       <c r="M2" s="96">
-        <f>L2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0478832949140027</v>
+        <f>$B$2*'DV-CAGR'!P91/'DV-CAGR'!$E$91</f>
+        <v>1.0464691756093496</v>
       </c>
       <c r="N2" s="96">
-        <f>M2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0523484017649856</v>
+        <f>$B$2*'DV-CAGR'!Q91/'DV-CAGR'!$E$91</f>
+        <v>1.0506936461192904</v>
       </c>
       <c r="O2" s="96">
-        <f>N2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0568325347606617</v>
+        <f>$B$2*'DV-CAGR'!R91/'DV-CAGR'!$E$91</f>
+        <v>1.0549181166292314</v>
       </c>
       <c r="P2" s="96">
-        <f>O2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0613357749728161</v>
+        <f>$B$2*'DV-CAGR'!S91/'DV-CAGR'!$E$91</f>
+        <v>1.0591425871391722</v>
       </c>
       <c r="Q2" s="96">
-        <f>P2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0658582038186861</v>
+        <f>$B$2*'DV-CAGR'!T91/'DV-CAGR'!$E$91</f>
+        <v>1.063367057649113</v>
       </c>
       <c r="R2" s="96">
-        <f>Q2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0703999030624343</v>
+        <f>$B$2*'DV-CAGR'!U91/'DV-CAGR'!$E$91</f>
+        <v>1.067591528159054</v>
       </c>
       <c r="S2" s="96">
-        <f>R2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0749609548166259</v>
+        <f>$B$2*'DV-CAGR'!V91/'DV-CAGR'!$E$91</f>
+        <v>1.0718159986689948</v>
       </c>
       <c r="T2" s="96">
-        <f>S2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0795414415437141</v>
+        <f>$B$2*'DV-CAGR'!W91/'DV-CAGR'!$E$91</f>
+        <v>1.0760404691789358</v>
       </c>
       <c r="U2" s="96">
-        <f>T2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0841414460575303</v>
+        <f>$B$2*'DV-CAGR'!X91/'DV-CAGR'!$E$91</f>
+        <v>1.0802649396888766</v>
       </c>
       <c r="V2" s="96">
-        <f>U2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0887610515247816</v>
+        <f>$B$2*'DV-CAGR'!Y91/'DV-CAGR'!$E$91</f>
+        <v>1.0844894101988174</v>
       </c>
       <c r="W2" s="96">
-        <f>V2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.093400341466555</v>
+        <f>$B$2*'DV-CAGR'!Z91/'DV-CAGR'!$E$91</f>
+        <v>1.0887138807087584</v>
       </c>
       <c r="X2" s="96">
-        <f>W2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.0980593997598262</v>
+        <f>$B$2*'DV-CAGR'!AA91/'DV-CAGR'!$E$91</f>
+        <v>1.0929383512186992</v>
       </c>
       <c r="Y2" s="96">
-        <f>X2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1027383106389774</v>
+        <f>$B$2*'DV-CAGR'!AB91/'DV-CAGR'!$E$91</f>
+        <v>1.09716282172864</v>
       </c>
       <c r="Z2" s="96">
-        <f>Y2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1074371586973193</v>
+        <f>$B$2*'DV-CAGR'!AC91/'DV-CAGR'!$E$91</f>
+        <v>1.101387292238581</v>
       </c>
       <c r="AA2" s="96">
-        <f>Z2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1121560288886208</v>
+        <f>$B$2*'DV-CAGR'!AD91/'DV-CAGR'!$E$91</f>
+        <v>1.1056117627485218</v>
       </c>
       <c r="AB2" s="96">
-        <f>AA2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1168950065286452</v>
+        <f>$B$2*'DV-CAGR'!AE91/'DV-CAGR'!$E$91</f>
+        <v>1.1098362332584626</v>
       </c>
       <c r="AC2" s="96">
-        <f>AB2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1216541772966924</v>
+        <f>$B$2*'DV-CAGR'!AF91/'DV-CAGR'!$E$91</f>
+        <v>1.1140607037684036</v>
       </c>
       <c r="AD2" s="96">
-        <f>AC2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.126433627237148</v>
+        <f>$B$2*'DV-CAGR'!AG91/'DV-CAGR'!$E$91</f>
+        <v>1.1182851742783444</v>
       </c>
       <c r="AE2" s="96">
-        <f>AD2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1312334427610389</v>
+        <f>$B$2*'DV-CAGR'!AH91/'DV-CAGR'!$E$91</f>
+        <v>1.1225096447882854</v>
       </c>
       <c r="AF2" s="96">
-        <f>AE2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1360537106475959</v>
+        <f>$B$2*'DV-CAGR'!AI91/'DV-CAGR'!$E$91</f>
+        <v>1.1267341152982262</v>
       </c>
       <c r="AG2" s="96">
-        <f>AF2*(1+'DV-CAGR'!$N$84)</f>
-        <v>1.1408945180458219</v>
+        <f>$B$2*'DV-CAGR'!AJ91/'DV-CAGR'!$E$91</f>
+        <v>1.130958585808167</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="95" customFormat="1">
@@ -29205,128 +29245,128 @@
         <v>1</v>
       </c>
       <c r="C3" s="96">
-        <f>B3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.0238834681230935</v>
+        <f>$B$3*'DV-CAGR'!F92/'DV-CAGR'!$E$92</f>
+        <v>1.021435057437267</v>
       </c>
       <c r="D3" s="96">
-        <f>C3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.0483373562957738</v>
+        <f>$B$3*'DV-CAGR'!G92/'DV-CAGR'!$E$92</f>
+        <v>1.0428701148745341</v>
       </c>
       <c r="E3" s="96">
-        <f>D3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.0733752881271121</v>
+        <f>$B$3*'DV-CAGR'!H92/'DV-CAGR'!$E$92</f>
+        <v>1.0643051723118011</v>
       </c>
       <c r="F3" s="96">
-        <f>E3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.0990112126052123</v>
+        <f>$B$3*'DV-CAGR'!I92/'DV-CAGR'!$E$92</f>
+        <v>1.0857402297490681</v>
       </c>
       <c r="G3" s="96">
-        <f>F3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.1252594118683912</v>
+        <f>$B$3*'DV-CAGR'!J92/'DV-CAGR'!$E$92</f>
+        <v>1.107175287186335</v>
       </c>
       <c r="H3" s="96">
-        <f>G3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.1521345091619608</v>
+        <f>$B$3*'DV-CAGR'!K92/'DV-CAGR'!$E$92</f>
+        <v>1.128610344623602</v>
       </c>
       <c r="I3" s="96">
-        <f>H3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.1796514769850466</v>
+        <f>$B$3*'DV-CAGR'!L92/'DV-CAGR'!$E$92</f>
+        <v>1.150045402060869</v>
       </c>
       <c r="J3" s="96">
-        <f>I3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.2078256454319791</v>
+        <f>$B$3*'DV-CAGR'!M92/'DV-CAGR'!$E$92</f>
+        <v>1.1714804594981361</v>
       </c>
       <c r="K3" s="96">
-        <f>J3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.2366727107329085</v>
+        <f>$B$3*'DV-CAGR'!N92/'DV-CAGR'!$E$92</f>
+        <v>1.1929155169354031</v>
       </c>
       <c r="L3" s="96">
-        <f>K3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.2662087439983976</v>
+        <f>$B$3*'DV-CAGR'!O92/'DV-CAGR'!$E$92</f>
+        <v>1.2143505743726701</v>
       </c>
       <c r="M3" s="96">
-        <f>L3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.2964502001728655</v>
+        <f>$B$3*'DV-CAGR'!P92/'DV-CAGR'!$E$92</f>
+        <v>1.2357856318099372</v>
       </c>
       <c r="N3" s="96">
-        <f>M3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.3274139272018723</v>
+        <f>$B$3*'DV-CAGR'!Q92/'DV-CAGR'!$E$92</f>
+        <v>1.257220689247204</v>
       </c>
       <c r="O3" s="96">
-        <f>N3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.3591171754183486</v>
+        <f>$B$3*'DV-CAGR'!R92/'DV-CAGR'!$E$92</f>
+        <v>1.278655746684471</v>
       </c>
       <c r="P3" s="96">
-        <f>O3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.3915776071530017</v>
+        <f>$B$3*'DV-CAGR'!S92/'DV-CAGR'!$E$92</f>
+        <v>1.3000908041217381</v>
       </c>
       <c r="Q3" s="96">
-        <f>P3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.4248133065742512</v>
+        <f>$B$3*'DV-CAGR'!T92/'DV-CAGR'!$E$92</f>
+        <v>1.3215258615590051</v>
       </c>
       <c r="R3" s="96">
-        <f>Q3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.4588427897631768</v>
+        <f>$B$3*'DV-CAGR'!U92/'DV-CAGR'!$E$92</f>
+        <v>1.3429609189962721</v>
       </c>
       <c r="S3" s="96">
-        <f>R3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.4936850150290903</v>
+        <f>$B$3*'DV-CAGR'!V92/'DV-CAGR'!$E$92</f>
+        <v>1.3643959764335392</v>
       </c>
       <c r="T3" s="96">
-        <f>S3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.52935939347148</v>
+        <f>$B$3*'DV-CAGR'!W92/'DV-CAGR'!$E$92</f>
+        <v>1.3858310338708062</v>
       </c>
       <c r="U3" s="96">
-        <f>T3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.5658857997942097</v>
+        <f>$B$3*'DV-CAGR'!X92/'DV-CAGR'!$E$92</f>
+        <v>1.4072660913080732</v>
       </c>
       <c r="V3" s="96">
-        <f>U3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.6032845833779994</v>
+        <f>$B$3*'DV-CAGR'!Y92/'DV-CAGR'!$E$92</f>
+        <v>1.4287011487453403</v>
       </c>
       <c r="W3" s="96">
-        <f>V3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.6415765796173551</v>
+        <f>$B$3*'DV-CAGR'!Z92/'DV-CAGR'!$E$92</f>
+        <v>1.4501362061826073</v>
       </c>
       <c r="X3" s="96">
-        <f>W3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.6807831215282631</v>
+        <f>$B$3*'DV-CAGR'!AA92/'DV-CAGR'!$E$92</f>
+        <v>1.4715712636198743</v>
       </c>
       <c r="Y3" s="96">
-        <f>X3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.7209260516331171</v>
+        <f>$B$3*'DV-CAGR'!AB92/'DV-CAGR'!$E$92</f>
+        <v>1.4930063210571412</v>
       </c>
       <c r="Z3" s="96">
-        <f>Y3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.7620277341294979</v>
+        <f>$B$3*'DV-CAGR'!AC92/'DV-CAGR'!$E$92</f>
+        <v>1.5144413784944082</v>
       </c>
       <c r="AA3" s="96">
-        <f>Z3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.8041110673495864</v>
+        <f>$B$3*'DV-CAGR'!AD92/'DV-CAGR'!$E$92</f>
+        <v>1.5358764359316752</v>
       </c>
       <c r="AB3" s="96">
-        <f>AA3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.8471994965171503</v>
+        <f>$B$3*'DV-CAGR'!AE92/'DV-CAGR'!$E$92</f>
+        <v>1.5573114933689423</v>
       </c>
       <c r="AC3" s="96">
-        <f>AB3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.8913170268092121</v>
+        <f>$B$3*'DV-CAGR'!AF92/'DV-CAGR'!$E$92</f>
+        <v>1.5787465508062093</v>
       </c>
       <c r="AD3" s="96">
-        <f>AC3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.9364882367296739</v>
+        <f>$B$3*'DV-CAGR'!AG92/'DV-CAGR'!$E$92</f>
+        <v>1.6001816082434763</v>
       </c>
       <c r="AE3" s="96">
-        <f>AD3*(1+'DV-CAGR'!$N$85)</f>
-        <v>1.9827382918023526</v>
+        <f>$B$3*'DV-CAGR'!AH92/'DV-CAGR'!$E$92</f>
+        <v>1.6216166656807434</v>
       </c>
       <c r="AF3" s="96">
-        <f>AE3*(1+'DV-CAGR'!$N$85)</f>
-        <v>2.0300929585910508</v>
+        <f>$B$3*'DV-CAGR'!AI92/'DV-CAGR'!$E$92</f>
+        <v>1.6430517231180104</v>
       </c>
       <c r="AG3" s="96">
-        <f>AF3*(1+'DV-CAGR'!$N$85)</f>
-        <v>2.0785786190544768</v>
+        <f>$B$3*'DV-CAGR'!AJ92/'DV-CAGR'!$E$92</f>
+        <v>1.6644867805552774</v>
       </c>
     </row>
     <row r="4" spans="1:33" s="95" customFormat="1">
@@ -29881,40 +29921,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
     </row>
     <row r="2" spans="1:8" ht="25.5">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="181" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="180" t="s">
+      <c r="B2" s="181" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="180" t="s">
+      <c r="C2" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="180" t="s">
+      <c r="D2" s="181" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="183" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="183"/>
+      <c r="G2" s="184"/>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A3" s="191"/>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
+      <c r="A3" s="192"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
       <c r="E3" s="36" t="s">
         <v>11</v>
       </c>
@@ -29929,7 +29969,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" thickTop="1">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="188" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="35" t="s">
@@ -29948,10 +29988,10 @@
       <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="188" t="s">
+      <c r="A5" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="184" t="s">
+      <c r="B5" s="185" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="25" t="s">
@@ -29967,13 +30007,13 @@
       <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="188" t="s">
+      <c r="A6" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="184" t="s">
+      <c r="B6" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="189" t="s">
+      <c r="C6" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="25" t="s">
@@ -29986,13 +30026,13 @@
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="188" t="s">
+      <c r="A7" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="184" t="s">
+      <c r="B7" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="189" t="s">
+      <c r="C7" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="25" t="s">
@@ -30011,13 +30051,13 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="188" t="s">
+      <c r="A8" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="184" t="s">
+      <c r="B8" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="189" t="s">
+      <c r="C8" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="25" t="s">
@@ -30033,13 +30073,13 @@
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="188" t="s">
+      <c r="A9" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="184" t="s">
+      <c r="B9" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="189" t="s">
+      <c r="C9" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -30055,13 +30095,13 @@
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="188" t="s">
+      <c r="A10" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="184" t="s">
+      <c r="B10" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="189" t="s">
+      <c r="C10" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="25" t="s">
@@ -30077,13 +30117,13 @@
       <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="188" t="s">
+      <c r="A11" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="184" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="189" t="s">
+      <c r="C11" s="190" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="25" t="s">
@@ -30096,13 +30136,13 @@
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="188" t="s">
+      <c r="A12" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="184" t="s">
+      <c r="B12" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="189" t="s">
+      <c r="C12" s="190" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="25" t="s">
@@ -30121,13 +30161,13 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="188" t="s">
+      <c r="A13" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="189" t="s">
+      <c r="C13" s="190" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="25" t="s">
@@ -30143,10 +30183,10 @@
       <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="188" t="s">
+      <c r="A14" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="184" t="s">
+      <c r="B14" s="185" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="25" t="s">
@@ -30168,10 +30208,10 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="188" t="s">
+      <c r="A15" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="184" t="s">
+      <c r="B15" s="185" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -30187,13 +30227,13 @@
       <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="188" t="s">
+      <c r="A16" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="184" t="s">
+      <c r="B16" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="189" t="s">
+      <c r="C16" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="25" t="s">
@@ -30206,13 +30246,13 @@
       <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="188" t="s">
+      <c r="A17" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="184" t="s">
+      <c r="B17" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="189" t="s">
+      <c r="C17" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="25" t="s">
@@ -30231,13 +30271,13 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="188" t="s">
+      <c r="A18" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="184" t="s">
+      <c r="B18" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="189" t="s">
+      <c r="C18" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="25" t="s">
@@ -30253,13 +30293,13 @@
       <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="188" t="s">
+      <c r="A19" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="184" t="s">
+      <c r="B19" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="189" t="s">
+      <c r="C19" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="25" t="s">
@@ -30275,10 +30315,10 @@
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A20" s="188" t="s">
+      <c r="A20" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="185" t="s">
+      <c r="B20" s="186" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="31" t="s">
@@ -30300,10 +30340,10 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="188" t="s">
+      <c r="A21" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="190" t="s">
+      <c r="B21" s="191" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="27" t="s">
@@ -30319,13 +30359,13 @@
       <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="188" t="s">
+      <c r="A22" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="184" t="s">
+      <c r="B22" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="189" t="s">
+      <c r="C22" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -30338,13 +30378,13 @@
       <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="188" t="s">
+      <c r="A23" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="184" t="s">
+      <c r="B23" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="189" t="s">
+      <c r="C23" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="25" t="s">
@@ -30363,13 +30403,13 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="188" t="s">
+      <c r="A24" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="184" t="s">
+      <c r="B24" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="189" t="s">
+      <c r="C24" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="25" t="s">
@@ -30385,13 +30425,13 @@
       <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="188" t="s">
+      <c r="A25" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="184" t="s">
+      <c r="B25" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="189" t="s">
+      <c r="C25" s="190" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="25" t="s">
@@ -30407,13 +30447,13 @@
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="188" t="s">
+      <c r="A26" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="184" t="s">
+      <c r="B26" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="189" t="s">
+      <c r="C26" s="190" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="25" t="s">
@@ -30426,13 +30466,13 @@
       <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="188" t="s">
+      <c r="A27" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="184" t="s">
+      <c r="B27" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="189" t="s">
+      <c r="C27" s="190" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="25" t="s">
@@ -30451,13 +30491,13 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="188" t="s">
+      <c r="A28" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="184" t="s">
+      <c r="B28" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="189" t="s">
+      <c r="C28" s="190" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="25" t="s">
@@ -30473,13 +30513,13 @@
       <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="188" t="s">
+      <c r="A29" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="184" t="s">
+      <c r="B29" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="189" t="s">
+      <c r="C29" s="190" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="25" t="s">
@@ -30495,13 +30535,13 @@
       <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="188" t="s">
+      <c r="A30" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="184" t="s">
+      <c r="B30" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="189" t="s">
+      <c r="C30" s="190" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="25" t="s">
@@ -30514,13 +30554,13 @@
       <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="188" t="s">
+      <c r="A31" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="184" t="s">
+      <c r="B31" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="189" t="s">
+      <c r="C31" s="190" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="25" t="s">
@@ -30542,13 +30582,13 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="188" t="s">
+      <c r="A32" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="184" t="s">
+      <c r="B32" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="189" t="s">
+      <c r="C32" s="190" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -30564,10 +30604,10 @@
       <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="188" t="s">
+      <c r="A33" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="184" t="s">
+      <c r="B33" s="185" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="25" t="s">
@@ -30589,10 +30629,10 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="188" t="s">
+      <c r="A34" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="184" t="s">
+      <c r="B34" s="185" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="25" t="s">
@@ -30608,10 +30648,10 @@
       <c r="G34" s="30"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="188" t="s">
+      <c r="A35" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="184" t="s">
+      <c r="B35" s="185" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="25" t="s">
@@ -30633,10 +30673,10 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="188" t="s">
+      <c r="A36" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="184" t="s">
+      <c r="B36" s="185" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="25" t="s">
@@ -30658,10 +30698,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A37" s="188" t="s">
+      <c r="A37" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="185" t="s">
+      <c r="B37" s="186" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="31" t="s">
@@ -30692,11 +30732,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B34:B37"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:A37"/>
     <mergeCell ref="B5:B14"/>
@@ -30709,6 +30744,11 @@
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B34:B37"/>
   </mergeCells>
   <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30718,10 +30758,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8691AF6E-6FF3-4258-B536-2AC6D3469E02}">
-  <dimension ref="A1:O85"/>
+  <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+      <selection activeCell="F89" sqref="F89:AJ92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -30738,16 +30778,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="197" t="s">
         <v>716</v>
       </c>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="195" t="s">
+      <c r="C1" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="195" t="s">
+      <c r="D1" s="197" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="116" t="s">
@@ -30779,16 +30819,16 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="198" t="s">
         <v>716</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="198" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="196" t="s">
+      <c r="C2" s="198" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="196" t="s">
+      <c r="D2" s="198" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="116" t="s">
@@ -30818,21 +30858,21 @@
       <c r="M2" s="171" t="s">
         <v>717</v>
       </c>
-      <c r="N2" s="197" t="s">
+      <c r="N2" s="193" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="198" t="s">
         <v>716</v>
       </c>
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="198" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="196" t="s">
+      <c r="C3" s="198" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="196" t="s">
+      <c r="D3" s="198" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="116" t="s">
@@ -30862,7 +30902,7 @@
       <c r="M3" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="197"/>
+      <c r="N3" s="193"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="120" t="s">
@@ -32467,10 +32507,10 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="100" customFormat="1">
-      <c r="C40" s="199" t="s">
+      <c r="C40" s="200" t="s">
         <v>781</v>
       </c>
-      <c r="D40" s="199"/>
+      <c r="D40" s="200"/>
       <c r="E40" s="113">
         <f>E23</f>
         <v>43.7</v>
@@ -32513,8 +32553,8 @@
       </c>
     </row>
     <row r="41" spans="1:15" s="100" customFormat="1">
-      <c r="C41" s="199"/>
-      <c r="D41" s="199"/>
+      <c r="C41" s="200"/>
+      <c r="D41" s="200"/>
       <c r="E41" s="113">
         <f>E24</f>
         <v>53.3</v>
@@ -32557,8 +32597,8 @@
       </c>
     </row>
     <row r="42" spans="1:15" s="100" customFormat="1">
-      <c r="C42" s="199"/>
-      <c r="D42" s="199"/>
+      <c r="C42" s="200"/>
+      <c r="D42" s="200"/>
       <c r="E42" s="113">
         <f>E27</f>
         <v>19.899999999999999</v>
@@ -32601,8 +32641,8 @@
       </c>
     </row>
     <row r="43" spans="1:15" s="100" customFormat="1">
-      <c r="C43" s="199"/>
-      <c r="D43" s="199"/>
+      <c r="C43" s="200"/>
+      <c r="D43" s="200"/>
       <c r="E43" s="113">
         <f>E28</f>
         <v>20.399999999999999</v>
@@ -32645,8 +32685,8 @@
       </c>
     </row>
     <row r="44" spans="1:15" s="100" customFormat="1">
-      <c r="C44" s="199"/>
-      <c r="D44" s="199"/>
+      <c r="C44" s="200"/>
+      <c r="D44" s="200"/>
       <c r="E44" s="113">
         <f>E31</f>
         <v>39.299999999999997</v>
@@ -32689,8 +32729,8 @@
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="C45" s="199"/>
-      <c r="D45" s="199"/>
+      <c r="C45" s="200"/>
+      <c r="D45" s="200"/>
       <c r="E45" s="113">
         <f>E32</f>
         <v>41.1</v>
@@ -32733,8 +32773,8 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="C46" s="199"/>
-      <c r="D46" s="199"/>
+      <c r="C46" s="200"/>
+      <c r="D46" s="200"/>
       <c r="E46" s="113">
         <f>E36</f>
         <v>60</v>
@@ -32781,10 +32821,10 @@
       <c r="N47" s="40"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="C48" s="199" t="s">
+      <c r="C48" s="200" t="s">
         <v>782</v>
       </c>
-      <c r="D48" s="199"/>
+      <c r="D48" s="200"/>
       <c r="E48" s="113">
         <f t="shared" ref="E48:N48" si="14">E25</f>
         <v>130.9</v>
@@ -32827,8 +32867,8 @@
       </c>
     </row>
     <row r="49" spans="1:14" s="100" customFormat="1">
-      <c r="C49" s="199"/>
-      <c r="D49" s="199"/>
+      <c r="C49" s="200"/>
+      <c r="D49" s="200"/>
       <c r="E49" s="113">
         <f t="shared" ref="E49:N49" si="15">E29</f>
         <v>21.5</v>
@@ -32871,8 +32911,8 @@
       </c>
     </row>
     <row r="50" spans="1:14" s="100" customFormat="1">
-      <c r="C50" s="199"/>
-      <c r="D50" s="199"/>
+      <c r="C50" s="200"/>
+      <c r="D50" s="200"/>
       <c r="E50" s="113">
         <f t="shared" ref="E50:N50" si="16">E33</f>
         <v>56.7</v>
@@ -32915,8 +32955,8 @@
       </c>
     </row>
     <row r="51" spans="1:14" s="100" customFormat="1">
-      <c r="C51" s="199"/>
-      <c r="D51" s="199"/>
+      <c r="C51" s="200"/>
+      <c r="D51" s="200"/>
       <c r="E51" s="113">
         <f t="shared" ref="E51:N51" si="17">E35</f>
         <v>215.1</v>
@@ -32959,8 +32999,8 @@
       </c>
     </row>
     <row r="52" spans="1:14" s="100" customFormat="1">
-      <c r="C52" s="199"/>
-      <c r="D52" s="199"/>
+      <c r="C52" s="200"/>
+      <c r="D52" s="200"/>
       <c r="E52" s="113">
         <f t="shared" ref="E52:N52" si="18">E37</f>
         <v>28.7</v>
@@ -33049,7 +33089,7 @@
       </c>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="198" t="s">
+      <c r="A60" s="199" t="s">
         <v>783</v>
       </c>
       <c r="B60" s="132" t="s">
@@ -33101,7 +33141,7 @@
       </c>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="198"/>
+      <c r="A61" s="199"/>
       <c r="B61" s="135" t="s">
         <v>725</v>
       </c>
@@ -33151,7 +33191,7 @@
       </c>
     </row>
     <row r="62" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A62" s="198"/>
+      <c r="A62" s="199"/>
       <c r="B62" s="138" t="s">
         <v>726</v>
       </c>
@@ -33201,7 +33241,7 @@
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="198" t="s">
+      <c r="A63" s="199" t="s">
         <v>784</v>
       </c>
       <c r="B63" s="132" t="s">
@@ -33253,7 +33293,7 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="198"/>
+      <c r="A64" s="199"/>
       <c r="B64" s="135" t="s">
         <v>725</v>
       </c>
@@ -33303,7 +33343,7 @@
       </c>
     </row>
     <row r="65" spans="1:15">
-      <c r="A65" s="198"/>
+      <c r="A65" s="199"/>
       <c r="B65" s="135" t="s">
         <v>725</v>
       </c>
@@ -33353,7 +33393,7 @@
       </c>
     </row>
     <row r="66" spans="1:15">
-      <c r="A66" s="198"/>
+      <c r="A66" s="199"/>
       <c r="B66" s="135" t="s">
         <v>726</v>
       </c>
@@ -33403,7 +33443,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A67" s="198"/>
+      <c r="A67" s="199"/>
       <c r="B67" s="138" t="s">
         <v>726</v>
       </c>
@@ -33452,6 +33492,11 @@
         <v>34815</v>
       </c>
     </row>
+    <row r="70" spans="1:15">
+      <c r="B70" s="215" t="s">
+        <v>791</v>
+      </c>
+    </row>
     <row r="71" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="72" spans="1:15" ht="15.75" thickBot="1">
       <c r="B72" s="194" t="s">
@@ -33503,7 +33548,7 @@
       </c>
     </row>
     <row r="73" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B73" s="193"/>
+      <c r="B73" s="195"/>
       <c r="C73" s="139" t="s">
         <v>729</v>
       </c>
@@ -33550,7 +33595,7 @@
       </c>
     </row>
     <row r="74" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B74" s="192" t="s">
+      <c r="B74" s="196" t="s">
         <v>779</v>
       </c>
       <c r="C74" s="70" t="s">
@@ -33599,7 +33644,7 @@
       </c>
     </row>
     <row r="75" spans="1:15" s="100" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B75" s="193"/>
+      <c r="B75" s="195"/>
       <c r="C75" s="139" t="s">
         <v>729</v>
       </c>
@@ -33688,7 +33733,7 @@
       <c r="O77" s="48"/>
     </row>
     <row r="78" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B78" s="193"/>
+      <c r="B78" s="195"/>
       <c r="C78" s="139" t="s">
         <v>729</v>
       </c>
@@ -33727,7 +33772,7 @@
       <c r="O78" s="48"/>
     </row>
     <row r="79" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B79" s="192" t="s">
+      <c r="B79" s="196" t="s">
         <v>779</v>
       </c>
       <c r="C79" s="70" t="s">
@@ -33768,7 +33813,7 @@
       <c r="O79" s="48"/>
     </row>
     <row r="80" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B80" s="193"/>
+      <c r="B80" s="195"/>
       <c r="C80" s="139" t="s">
         <v>729</v>
       </c>
@@ -33806,7 +33851,7 @@
       </c>
       <c r="O80" s="48"/>
     </row>
-    <row r="81" spans="2:15" ht="15.75" thickBot="1">
+    <row r="81" spans="2:36" ht="15.75" thickBot="1">
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
       <c r="D81" s="48"/>
@@ -33820,9 +33865,11 @@
       <c r="L81" s="48"/>
       <c r="M81" s="48"/>
       <c r="N81" s="48"/>
-      <c r="O81" s="48"/>
-    </row>
-    <row r="82" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="O81" s="48" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="82" spans="2:36" ht="16.5" thickTop="1" thickBot="1">
       <c r="B82" s="194" t="s">
         <v>778</v>
       </c>
@@ -33870,10 +33917,13 @@
         <f>(M82/E82)^(1/8)-1</f>
         <v>2.5754463465193611E-2</v>
       </c>
-      <c r="O82" s="48"/>
-    </row>
-    <row r="83" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B83" s="193"/>
+      <c r="O82" s="48">
+        <f>(M82-E82)/8</f>
+        <v>1502.6593177948425</v>
+      </c>
+    </row>
+    <row r="83" spans="2:36" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B83" s="195"/>
       <c r="C83" s="139" t="s">
         <v>729</v>
       </c>
@@ -33918,10 +33968,13 @@
         <f t="shared" ref="N83" si="43">(M83/E83)^(1/8)-1</f>
         <v>-4.5194730002432681E-2</v>
       </c>
-      <c r="O83" s="48"/>
-    </row>
-    <row r="84" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B84" s="192" t="s">
+      <c r="O83" s="48">
+        <f t="shared" ref="O83:O85" si="44">(M83-E83)/8</f>
+        <v>-173.85632629554618</v>
+      </c>
+    </row>
+    <row r="84" spans="2:36" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B84" s="196" t="s">
         <v>779</v>
       </c>
       <c r="C84" s="70" t="s">
@@ -33929,95 +33982,752 @@
       </c>
       <c r="D84" s="133"/>
       <c r="E84" s="178">
-        <f t="shared" ref="E84:M84" si="44">E74*E79</f>
+        <f t="shared" ref="E84:M84" si="45">E74*E79</f>
         <v>14176.873480961749</v>
       </c>
       <c r="F84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>14298.968917874234</v>
       </c>
       <c r="G84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>14480.549757733557</v>
       </c>
       <c r="H84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>15005.30291161387</v>
       </c>
       <c r="I84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>15115.408033898173</v>
       </c>
       <c r="J84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>15448.667900609029</v>
       </c>
       <c r="K84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>15347.886968245761</v>
       </c>
       <c r="L84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>14514.795849424441</v>
       </c>
       <c r="M84" s="178">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>14667.412097151402</v>
       </c>
       <c r="N84" s="175">
         <f>(M84/E84)^(1/8)-1</f>
         <v>4.2610726525127429E-3</v>
       </c>
-    </row>
-    <row r="85" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B85" s="193"/>
+      <c r="O84" s="48">
+        <f t="shared" si="44"/>
+        <v>61.317327023706639</v>
+      </c>
+    </row>
+    <row r="85" spans="2:36" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B85" s="195"/>
       <c r="C85" s="139" t="s">
         <v>729</v>
       </c>
       <c r="D85" s="133"/>
       <c r="E85" s="178">
-        <f t="shared" ref="E85:M85" si="45">E75*E80</f>
+        <f t="shared" ref="E85:M85" si="46">E75*E80</f>
         <v>24788.778793767851</v>
       </c>
       <c r="F85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>25272.117646957464</v>
       </c>
       <c r="G85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>25666.975432524672</v>
       </c>
       <c r="H85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>26375.716124613384</v>
       </c>
       <c r="I85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>27278.881969656504</v>
       </c>
       <c r="J85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>28253.60517048063</v>
       </c>
       <c r="K85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>27613.033618093359</v>
       </c>
       <c r="L85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>30042.746371001984</v>
       </c>
       <c r="M85" s="178">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>29940.522746053222</v>
       </c>
       <c r="N85" s="176">
-        <f t="shared" ref="N85" si="46">(M85/E85)^(1/8)-1</f>
+        <f t="shared" ref="N85" si="47">(M85/E85)^(1/8)-1</f>
         <v>2.3883468123093499E-2</v>
       </c>
+      <c r="O85" s="48">
+        <f t="shared" si="44"/>
+        <v>643.96799403567138</v>
+      </c>
+    </row>
+    <row r="88" spans="2:36" ht="15.75" thickBot="1">
+      <c r="E88" s="99">
+        <v>2019</v>
+      </c>
+      <c r="F88" s="180">
+        <v>2020</v>
+      </c>
+      <c r="G88" s="180">
+        <v>2021</v>
+      </c>
+      <c r="H88" s="180">
+        <v>2022</v>
+      </c>
+      <c r="I88" s="180">
+        <v>2023</v>
+      </c>
+      <c r="J88" s="180">
+        <v>2024</v>
+      </c>
+      <c r="K88" s="180">
+        <v>2025</v>
+      </c>
+      <c r="L88" s="180">
+        <v>2026</v>
+      </c>
+      <c r="M88" s="180">
+        <v>2027</v>
+      </c>
+      <c r="N88" s="180">
+        <v>2028</v>
+      </c>
+      <c r="O88" s="180">
+        <v>2029</v>
+      </c>
+      <c r="P88" s="180">
+        <v>2030</v>
+      </c>
+      <c r="Q88" s="180">
+        <v>2031</v>
+      </c>
+      <c r="R88" s="180">
+        <v>2032</v>
+      </c>
+      <c r="S88" s="180">
+        <v>2033</v>
+      </c>
+      <c r="T88" s="180">
+        <v>2034</v>
+      </c>
+      <c r="U88" s="180">
+        <v>2035</v>
+      </c>
+      <c r="V88" s="180">
+        <v>2036</v>
+      </c>
+      <c r="W88" s="180">
+        <v>2037</v>
+      </c>
+      <c r="X88" s="180">
+        <v>2038</v>
+      </c>
+      <c r="Y88" s="180">
+        <v>2039</v>
+      </c>
+      <c r="Z88" s="180">
+        <v>2040</v>
+      </c>
+      <c r="AA88" s="180">
+        <v>2041</v>
+      </c>
+      <c r="AB88" s="180">
+        <v>2042</v>
+      </c>
+      <c r="AC88" s="180">
+        <v>2043</v>
+      </c>
+      <c r="AD88" s="180">
+        <v>2044</v>
+      </c>
+      <c r="AE88" s="180">
+        <v>2045</v>
+      </c>
+      <c r="AF88" s="180">
+        <v>2046</v>
+      </c>
+      <c r="AG88" s="180">
+        <v>2047</v>
+      </c>
+      <c r="AH88" s="180">
+        <v>2048</v>
+      </c>
+      <c r="AI88" s="180">
+        <v>2049</v>
+      </c>
+      <c r="AJ88" s="180">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="89" spans="2:36" ht="15.75" thickBot="1">
+      <c r="B89" s="194" t="s">
+        <v>778</v>
+      </c>
+      <c r="C89" s="133" t="s">
+        <v>728</v>
+      </c>
+      <c r="D89" s="133"/>
+      <c r="E89" s="90">
+        <f>L82</f>
+        <v>64309.137872188789</v>
+      </c>
+      <c r="F89" s="90">
+        <f>E89+$O82</f>
+        <v>65811.797189983627</v>
+      </c>
+      <c r="G89" s="90">
+        <f t="shared" ref="G89:AJ92" si="48">F89+$O82</f>
+        <v>67314.456507778465</v>
+      </c>
+      <c r="H89" s="90">
+        <f t="shared" si="48"/>
+        <v>68817.115825573303</v>
+      </c>
+      <c r="I89" s="90">
+        <f t="shared" si="48"/>
+        <v>70319.775143368141</v>
+      </c>
+      <c r="J89" s="90">
+        <f t="shared" si="48"/>
+        <v>71822.434461162979</v>
+      </c>
+      <c r="K89" s="90">
+        <f t="shared" si="48"/>
+        <v>73325.093778957817</v>
+      </c>
+      <c r="L89" s="90">
+        <f t="shared" si="48"/>
+        <v>74827.753096752655</v>
+      </c>
+      <c r="M89" s="90">
+        <f t="shared" si="48"/>
+        <v>76330.412414547493</v>
+      </c>
+      <c r="N89" s="90">
+        <f t="shared" si="48"/>
+        <v>77833.071732342331</v>
+      </c>
+      <c r="O89" s="90">
+        <f t="shared" si="48"/>
+        <v>79335.731050137168</v>
+      </c>
+      <c r="P89" s="90">
+        <f t="shared" si="48"/>
+        <v>80838.390367932006</v>
+      </c>
+      <c r="Q89" s="90">
+        <f t="shared" si="48"/>
+        <v>82341.049685726844</v>
+      </c>
+      <c r="R89" s="90">
+        <f t="shared" si="48"/>
+        <v>83843.709003521682</v>
+      </c>
+      <c r="S89" s="90">
+        <f t="shared" si="48"/>
+        <v>85346.36832131652</v>
+      </c>
+      <c r="T89" s="90">
+        <f t="shared" si="48"/>
+        <v>86849.027639111358</v>
+      </c>
+      <c r="U89" s="90">
+        <f t="shared" si="48"/>
+        <v>88351.686956906196</v>
+      </c>
+      <c r="V89" s="90">
+        <f t="shared" si="48"/>
+        <v>89854.346274701034</v>
+      </c>
+      <c r="W89" s="90">
+        <f t="shared" si="48"/>
+        <v>91357.005592495872</v>
+      </c>
+      <c r="X89" s="90">
+        <f t="shared" si="48"/>
+        <v>92859.66491029071</v>
+      </c>
+      <c r="Y89" s="90">
+        <f t="shared" si="48"/>
+        <v>94362.324228085548</v>
+      </c>
+      <c r="Z89" s="90">
+        <f t="shared" si="48"/>
+        <v>95864.983545880386</v>
+      </c>
+      <c r="AA89" s="90">
+        <f t="shared" si="48"/>
+        <v>97367.642863675224</v>
+      </c>
+      <c r="AB89" s="90">
+        <f t="shared" si="48"/>
+        <v>98870.302181470062</v>
+      </c>
+      <c r="AC89" s="90">
+        <f t="shared" si="48"/>
+        <v>100372.9614992649</v>
+      </c>
+      <c r="AD89" s="90">
+        <f t="shared" si="48"/>
+        <v>101875.62081705974</v>
+      </c>
+      <c r="AE89" s="90">
+        <f t="shared" si="48"/>
+        <v>103378.28013485458</v>
+      </c>
+      <c r="AF89" s="90">
+        <f t="shared" si="48"/>
+        <v>104880.93945264941</v>
+      </c>
+      <c r="AG89" s="90">
+        <f t="shared" si="48"/>
+        <v>106383.59877044425</v>
+      </c>
+      <c r="AH89" s="90">
+        <f t="shared" si="48"/>
+        <v>107886.25808823909</v>
+      </c>
+      <c r="AI89" s="90">
+        <f t="shared" si="48"/>
+        <v>109388.91740603393</v>
+      </c>
+      <c r="AJ89" s="90">
+        <f t="shared" si="48"/>
+        <v>110891.57672382877</v>
+      </c>
+    </row>
+    <row r="90" spans="2:36" ht="15.75" thickBot="1">
+      <c r="B90" s="195"/>
+      <c r="C90" s="139" t="s">
+        <v>729</v>
+      </c>
+      <c r="D90" s="133"/>
+      <c r="E90" s="90">
+        <f t="shared" ref="E90:E92" si="49">L83</f>
+        <v>3276.6076353792082</v>
+      </c>
+      <c r="F90" s="90">
+        <f t="shared" ref="F90:U92" si="50">E90+$O83</f>
+        <v>3102.7513090836619</v>
+      </c>
+      <c r="G90" s="90">
+        <f t="shared" si="50"/>
+        <v>2928.8949827881156</v>
+      </c>
+      <c r="H90" s="90">
+        <f t="shared" si="50"/>
+        <v>2755.0386564925693</v>
+      </c>
+      <c r="I90" s="90">
+        <f t="shared" si="50"/>
+        <v>2581.182330197023</v>
+      </c>
+      <c r="J90" s="90">
+        <f t="shared" si="50"/>
+        <v>2407.3260039014767</v>
+      </c>
+      <c r="K90" s="90">
+        <f t="shared" si="50"/>
+        <v>2233.4696776059304</v>
+      </c>
+      <c r="L90" s="90">
+        <f t="shared" si="50"/>
+        <v>2059.6133513103841</v>
+      </c>
+      <c r="M90" s="90">
+        <f t="shared" si="50"/>
+        <v>1885.7570250148378</v>
+      </c>
+      <c r="N90" s="90">
+        <f t="shared" si="50"/>
+        <v>1711.9006987192915</v>
+      </c>
+      <c r="O90" s="90">
+        <f t="shared" si="50"/>
+        <v>1538.0443724237452</v>
+      </c>
+      <c r="P90" s="90">
+        <f t="shared" si="50"/>
+        <v>1364.1880461281989</v>
+      </c>
+      <c r="Q90" s="90">
+        <f t="shared" si="50"/>
+        <v>1190.3317198326527</v>
+      </c>
+      <c r="R90" s="90">
+        <f t="shared" si="50"/>
+        <v>1016.4753935371065</v>
+      </c>
+      <c r="S90" s="90">
+        <f t="shared" si="50"/>
+        <v>842.61906724156029</v>
+      </c>
+      <c r="T90" s="90">
+        <f t="shared" si="50"/>
+        <v>668.76274094601411</v>
+      </c>
+      <c r="U90" s="90">
+        <f t="shared" si="50"/>
+        <v>494.90641465046792</v>
+      </c>
+      <c r="V90" s="90">
+        <f t="shared" si="48"/>
+        <v>321.05008835492174</v>
+      </c>
+      <c r="W90" s="90">
+        <f t="shared" si="48"/>
+        <v>147.19376205937556</v>
+      </c>
+      <c r="X90" s="90">
+        <f t="shared" si="48"/>
+        <v>-26.662564236170624</v>
+      </c>
+      <c r="Y90" s="90">
+        <f t="shared" si="48"/>
+        <v>-200.51889053171681</v>
+      </c>
+      <c r="Z90" s="90">
+        <f t="shared" si="48"/>
+        <v>-374.37521682726299</v>
+      </c>
+      <c r="AA90" s="90">
+        <f t="shared" si="48"/>
+        <v>-548.23154312280917</v>
+      </c>
+      <c r="AB90" s="90">
+        <f t="shared" si="48"/>
+        <v>-722.08786941835535</v>
+      </c>
+      <c r="AC90" s="90">
+        <f t="shared" si="48"/>
+        <v>-895.94419571390154</v>
+      </c>
+      <c r="AD90" s="90">
+        <f t="shared" si="48"/>
+        <v>-1069.8005220094478</v>
+      </c>
+      <c r="AE90" s="90">
+        <f t="shared" si="48"/>
+        <v>-1243.6568483049941</v>
+      </c>
+      <c r="AF90" s="90">
+        <f t="shared" si="48"/>
+        <v>-1417.5131746005404</v>
+      </c>
+      <c r="AG90" s="90">
+        <f t="shared" si="48"/>
+        <v>-1591.3695008960867</v>
+      </c>
+      <c r="AH90" s="90">
+        <f t="shared" si="48"/>
+        <v>-1765.225827191633</v>
+      </c>
+      <c r="AI90" s="90">
+        <f t="shared" si="48"/>
+        <v>-1939.0821534871793</v>
+      </c>
+      <c r="AJ90" s="90">
+        <f t="shared" si="48"/>
+        <v>-2112.9384797827256</v>
+      </c>
+    </row>
+    <row r="91" spans="2:36" ht="15.75" thickBot="1">
+      <c r="B91" s="196" t="s">
+        <v>779</v>
+      </c>
+      <c r="C91" s="70" t="s">
+        <v>728</v>
+      </c>
+      <c r="D91" s="133"/>
+      <c r="E91" s="90">
+        <f t="shared" si="49"/>
+        <v>14514.795849424441</v>
+      </c>
+      <c r="F91" s="90">
+        <f t="shared" si="50"/>
+        <v>14576.113176448147</v>
+      </c>
+      <c r="G91" s="90">
+        <f t="shared" si="48"/>
+        <v>14637.430503471853</v>
+      </c>
+      <c r="H91" s="90">
+        <f t="shared" si="48"/>
+        <v>14698.747830495558</v>
+      </c>
+      <c r="I91" s="90">
+        <f t="shared" si="48"/>
+        <v>14760.065157519264</v>
+      </c>
+      <c r="J91" s="90">
+        <f t="shared" si="48"/>
+        <v>14821.38248454297</v>
+      </c>
+      <c r="K91" s="90">
+        <f t="shared" si="48"/>
+        <v>14882.699811566676</v>
+      </c>
+      <c r="L91" s="90">
+        <f t="shared" si="48"/>
+        <v>14944.017138590381</v>
+      </c>
+      <c r="M91" s="90">
+        <f t="shared" si="48"/>
+        <v>15005.334465614087</v>
+      </c>
+      <c r="N91" s="90">
+        <f t="shared" si="48"/>
+        <v>15066.651792637793</v>
+      </c>
+      <c r="O91" s="90">
+        <f t="shared" si="48"/>
+        <v>15127.969119661499</v>
+      </c>
+      <c r="P91" s="90">
+        <f t="shared" si="48"/>
+        <v>15189.286446685204</v>
+      </c>
+      <c r="Q91" s="90">
+        <f t="shared" si="48"/>
+        <v>15250.60377370891</v>
+      </c>
+      <c r="R91" s="90">
+        <f t="shared" si="48"/>
+        <v>15311.921100732616</v>
+      </c>
+      <c r="S91" s="90">
+        <f t="shared" si="48"/>
+        <v>15373.238427756321</v>
+      </c>
+      <c r="T91" s="90">
+        <f t="shared" si="48"/>
+        <v>15434.555754780027</v>
+      </c>
+      <c r="U91" s="90">
+        <f t="shared" si="48"/>
+        <v>15495.873081803733</v>
+      </c>
+      <c r="V91" s="90">
+        <f t="shared" si="48"/>
+        <v>15557.190408827439</v>
+      </c>
+      <c r="W91" s="90">
+        <f t="shared" si="48"/>
+        <v>15618.507735851144</v>
+      </c>
+      <c r="X91" s="90">
+        <f t="shared" si="48"/>
+        <v>15679.82506287485</v>
+      </c>
+      <c r="Y91" s="90">
+        <f t="shared" si="48"/>
+        <v>15741.142389898556</v>
+      </c>
+      <c r="Z91" s="90">
+        <f t="shared" si="48"/>
+        <v>15802.459716922262</v>
+      </c>
+      <c r="AA91" s="90">
+        <f t="shared" si="48"/>
+        <v>15863.777043945967</v>
+      </c>
+      <c r="AB91" s="90">
+        <f t="shared" si="48"/>
+        <v>15925.094370969673</v>
+      </c>
+      <c r="AC91" s="90">
+        <f t="shared" si="48"/>
+        <v>15986.411697993379</v>
+      </c>
+      <c r="AD91" s="90">
+        <f t="shared" si="48"/>
+        <v>16047.729025017084</v>
+      </c>
+      <c r="AE91" s="90">
+        <f t="shared" si="48"/>
+        <v>16109.04635204079</v>
+      </c>
+      <c r="AF91" s="90">
+        <f t="shared" si="48"/>
+        <v>16170.363679064496</v>
+      </c>
+      <c r="AG91" s="90">
+        <f t="shared" si="48"/>
+        <v>16231.681006088202</v>
+      </c>
+      <c r="AH91" s="90">
+        <f t="shared" si="48"/>
+        <v>16292.998333111907</v>
+      </c>
+      <c r="AI91" s="90">
+        <f t="shared" si="48"/>
+        <v>16354.315660135613</v>
+      </c>
+      <c r="AJ91" s="90">
+        <f t="shared" si="48"/>
+        <v>16415.632987159319</v>
+      </c>
+    </row>
+    <row r="92" spans="2:36" ht="15.75" thickBot="1">
+      <c r="B92" s="195"/>
+      <c r="C92" s="139" t="s">
+        <v>729</v>
+      </c>
+      <c r="D92" s="133"/>
+      <c r="E92" s="90">
+        <f t="shared" si="49"/>
+        <v>30042.746371001984</v>
+      </c>
+      <c r="F92" s="90">
+        <f t="shared" si="50"/>
+        <v>30686.714365037657</v>
+      </c>
+      <c r="G92" s="90">
+        <f t="shared" si="48"/>
+        <v>31330.682359073329</v>
+      </c>
+      <c r="H92" s="90">
+        <f t="shared" si="48"/>
+        <v>31974.650353109002</v>
+      </c>
+      <c r="I92" s="90">
+        <f t="shared" si="48"/>
+        <v>32618.618347144675</v>
+      </c>
+      <c r="J92" s="90">
+        <f t="shared" si="48"/>
+        <v>33262.586341180344</v>
+      </c>
+      <c r="K92" s="90">
+        <f t="shared" si="48"/>
+        <v>33906.554335216017</v>
+      </c>
+      <c r="L92" s="90">
+        <f t="shared" si="48"/>
+        <v>34550.522329251689</v>
+      </c>
+      <c r="M92" s="90">
+        <f t="shared" si="48"/>
+        <v>35194.490323287362</v>
+      </c>
+      <c r="N92" s="90">
+        <f t="shared" si="48"/>
+        <v>35838.458317323035</v>
+      </c>
+      <c r="O92" s="90">
+        <f t="shared" si="48"/>
+        <v>36482.426311358708</v>
+      </c>
+      <c r="P92" s="90">
+        <f t="shared" si="48"/>
+        <v>37126.39430539438</v>
+      </c>
+      <c r="Q92" s="90">
+        <f t="shared" si="48"/>
+        <v>37770.362299430053</v>
+      </c>
+      <c r="R92" s="90">
+        <f t="shared" si="48"/>
+        <v>38414.330293465726</v>
+      </c>
+      <c r="S92" s="90">
+        <f t="shared" si="48"/>
+        <v>39058.298287501399</v>
+      </c>
+      <c r="T92" s="90">
+        <f t="shared" si="48"/>
+        <v>39702.266281537071</v>
+      </c>
+      <c r="U92" s="90">
+        <f t="shared" si="48"/>
+        <v>40346.234275572744</v>
+      </c>
+      <c r="V92" s="90">
+        <f t="shared" si="48"/>
+        <v>40990.202269608417</v>
+      </c>
+      <c r="W92" s="90">
+        <f t="shared" si="48"/>
+        <v>41634.17026364409</v>
+      </c>
+      <c r="X92" s="90">
+        <f t="shared" si="48"/>
+        <v>42278.138257679762</v>
+      </c>
+      <c r="Y92" s="90">
+        <f t="shared" si="48"/>
+        <v>42922.106251715435</v>
+      </c>
+      <c r="Z92" s="90">
+        <f t="shared" si="48"/>
+        <v>43566.074245751108</v>
+      </c>
+      <c r="AA92" s="90">
+        <f t="shared" si="48"/>
+        <v>44210.042239786781</v>
+      </c>
+      <c r="AB92" s="90">
+        <f t="shared" si="48"/>
+        <v>44854.010233822453</v>
+      </c>
+      <c r="AC92" s="90">
+        <f t="shared" si="48"/>
+        <v>45497.978227858126</v>
+      </c>
+      <c r="AD92" s="90">
+        <f t="shared" si="48"/>
+        <v>46141.946221893799</v>
+      </c>
+      <c r="AE92" s="90">
+        <f t="shared" si="48"/>
+        <v>46785.914215929472</v>
+      </c>
+      <c r="AF92" s="90">
+        <f t="shared" si="48"/>
+        <v>47429.882209965144</v>
+      </c>
+      <c r="AG92" s="90">
+        <f t="shared" si="48"/>
+        <v>48073.850204000817</v>
+      </c>
+      <c r="AH92" s="90">
+        <f t="shared" si="48"/>
+        <v>48717.81819803649</v>
+      </c>
+      <c r="AI92" s="90">
+        <f t="shared" si="48"/>
+        <v>49361.786192072163</v>
+      </c>
+      <c r="AJ92" s="90">
+        <f t="shared" si="48"/>
+        <v>50005.754186107835</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="D1:D3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="B74:B75"/>
@@ -34028,11 +34738,6 @@
     <mergeCell ref="A63:A67"/>
     <mergeCell ref="C40:D46"/>
     <mergeCell ref="C48:D52"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="D1:D3"/>
   </mergeCells>
   <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34053,29 +34758,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
+      <c r="O1" s="202"/>
+      <c r="P1" s="202"/>
+      <c r="Q1" s="202"/>
+      <c r="R1" s="202"/>
+      <c r="S1" s="202"/>
+      <c r="T1" s="202"/>
+      <c r="U1" s="202"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="85" t="s">
@@ -34988,28 +35693,28 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="202" t="s">
+      <c r="A18" s="203" t="s">
         <v>419</v>
       </c>
-      <c r="B18" s="201"/>
-      <c r="C18" s="201"/>
-      <c r="D18" s="201"/>
-      <c r="E18" s="201"/>
-      <c r="F18" s="201"/>
-      <c r="G18" s="201"/>
-      <c r="H18" s="201"/>
-      <c r="I18" s="201"/>
-      <c r="J18" s="201"/>
-      <c r="K18" s="201"/>
-      <c r="L18" s="201"/>
-      <c r="M18" s="201"/>
-      <c r="N18" s="201"/>
-      <c r="O18" s="201"/>
-      <c r="P18" s="201"/>
-      <c r="Q18" s="201"/>
-      <c r="R18" s="201"/>
-      <c r="S18" s="201"/>
-      <c r="T18" s="201"/>
+      <c r="B18" s="202"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="202"/>
+      <c r="F18" s="202"/>
+      <c r="G18" s="202"/>
+      <c r="H18" s="202"/>
+      <c r="I18" s="202"/>
+      <c r="J18" s="202"/>
+      <c r="K18" s="202"/>
+      <c r="L18" s="202"/>
+      <c r="M18" s="202"/>
+      <c r="N18" s="202"/>
+      <c r="O18" s="202"/>
+      <c r="P18" s="202"/>
+      <c r="Q18" s="202"/>
+      <c r="R18" s="202"/>
+      <c r="S18" s="202"/>
+      <c r="T18" s="202"/>
       <c r="U18" s="87">
         <v>44452.597080150474</v>
       </c>
@@ -35038,29 +35743,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
+      <c r="O1" s="202"/>
+      <c r="P1" s="202"/>
+      <c r="Q1" s="202"/>
+      <c r="R1" s="202"/>
+      <c r="S1" s="202"/>
+      <c r="T1" s="202"/>
+      <c r="U1" s="202"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="85" t="s">
@@ -35973,28 +36678,28 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="202" t="s">
+      <c r="A18" s="203" t="s">
         <v>419</v>
       </c>
-      <c r="B18" s="201"/>
-      <c r="C18" s="201"/>
-      <c r="D18" s="201"/>
-      <c r="E18" s="201"/>
-      <c r="F18" s="201"/>
-      <c r="G18" s="201"/>
-      <c r="H18" s="201"/>
-      <c r="I18" s="201"/>
-      <c r="J18" s="201"/>
-      <c r="K18" s="201"/>
-      <c r="L18" s="201"/>
-      <c r="M18" s="201"/>
-      <c r="N18" s="201"/>
-      <c r="O18" s="201"/>
-      <c r="P18" s="201"/>
-      <c r="Q18" s="201"/>
-      <c r="R18" s="201"/>
-      <c r="S18" s="201"/>
-      <c r="T18" s="201"/>
+      <c r="B18" s="202"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="202"/>
+      <c r="F18" s="202"/>
+      <c r="G18" s="202"/>
+      <c r="H18" s="202"/>
+      <c r="I18" s="202"/>
+      <c r="J18" s="202"/>
+      <c r="K18" s="202"/>
+      <c r="L18" s="202"/>
+      <c r="M18" s="202"/>
+      <c r="N18" s="202"/>
+      <c r="O18" s="202"/>
+      <c r="P18" s="202"/>
+      <c r="Q18" s="202"/>
+      <c r="R18" s="202"/>
+      <c r="S18" s="202"/>
+      <c r="T18" s="202"/>
       <c r="U18" s="87">
         <v>44452.596946840291</v>
       </c>
@@ -36023,29 +36728,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
+      <c r="O1" s="202"/>
+      <c r="P1" s="202"/>
+      <c r="Q1" s="202"/>
+      <c r="R1" s="202"/>
+      <c r="S1" s="202"/>
+      <c r="T1" s="202"/>
+      <c r="U1" s="202"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="85" t="s">
@@ -36633,28 +37338,28 @@
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="202" t="s">
+      <c r="A13" s="203" t="s">
         <v>419</v>
       </c>
-      <c r="B13" s="201"/>
-      <c r="C13" s="201"/>
-      <c r="D13" s="201"/>
-      <c r="E13" s="201"/>
-      <c r="F13" s="201"/>
-      <c r="G13" s="201"/>
-      <c r="H13" s="201"/>
-      <c r="I13" s="201"/>
-      <c r="J13" s="201"/>
-      <c r="K13" s="201"/>
-      <c r="L13" s="201"/>
-      <c r="M13" s="201"/>
-      <c r="N13" s="201"/>
-      <c r="O13" s="201"/>
-      <c r="P13" s="201"/>
-      <c r="Q13" s="201"/>
-      <c r="R13" s="201"/>
-      <c r="S13" s="201"/>
-      <c r="T13" s="201"/>
+      <c r="B13" s="202"/>
+      <c r="C13" s="202"/>
+      <c r="D13" s="202"/>
+      <c r="E13" s="202"/>
+      <c r="F13" s="202"/>
+      <c r="G13" s="202"/>
+      <c r="H13" s="202"/>
+      <c r="I13" s="202"/>
+      <c r="J13" s="202"/>
+      <c r="K13" s="202"/>
+      <c r="L13" s="202"/>
+      <c r="M13" s="202"/>
+      <c r="N13" s="202"/>
+      <c r="O13" s="202"/>
+      <c r="P13" s="202"/>
+      <c r="Q13" s="202"/>
+      <c r="R13" s="202"/>
+      <c r="S13" s="202"/>
+      <c r="T13" s="202"/>
       <c r="U13" s="87">
         <v>44452.596521967585</v>
       </c>
@@ -36683,19 +37388,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="85" t="s">
@@ -37223,18 +37928,18 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="202" t="s">
+      <c r="A19" s="203" t="s">
         <v>419</v>
       </c>
-      <c r="B19" s="201"/>
-      <c r="C19" s="201"/>
-      <c r="D19" s="201"/>
-      <c r="E19" s="201"/>
-      <c r="F19" s="201"/>
-      <c r="G19" s="201"/>
-      <c r="H19" s="201"/>
-      <c r="I19" s="201"/>
-      <c r="J19" s="201"/>
+      <c r="B19" s="202"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
       <c r="K19" s="87">
         <v>44452.580671828706</v>
       </c>
@@ -37268,19 +37973,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="85" t="s">
@@ -37808,18 +38513,18 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="202" t="s">
+      <c r="A19" s="203" t="s">
         <v>419</v>
       </c>
-      <c r="B19" s="201"/>
-      <c r="C19" s="201"/>
-      <c r="D19" s="201"/>
-      <c r="E19" s="201"/>
-      <c r="F19" s="201"/>
-      <c r="G19" s="201"/>
-      <c r="H19" s="201"/>
-      <c r="I19" s="201"/>
-      <c r="J19" s="201"/>
+      <c r="B19" s="202"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
       <c r="K19" s="87">
         <v>44452.580602870381</v>
       </c>

</xml_diff>